<commit_message>
create social publish and worked the painel_covid
</commit_message>
<xml_diff>
--- a/data/dados_Juazeiro_BA.xlsx
+++ b/data/dados_Juazeiro_BA.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="371">
-  <si>
-    <t>confirmados</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="469">
+  <si>
+    <t>casos</t>
   </si>
   <si>
     <t>mortos</t>
@@ -34,1099 +34,1393 @@
     <t>date</t>
   </si>
   <si>
-    <t>23/mar</t>
-  </si>
-  <si>
-    <t>24/mar</t>
-  </si>
-  <si>
-    <t>25/mar</t>
-  </si>
-  <si>
-    <t>26/mar</t>
-  </si>
-  <si>
-    <t>27/mar</t>
-  </si>
-  <si>
-    <t>28/mar</t>
-  </si>
-  <si>
-    <t>29/mar</t>
-  </si>
-  <si>
-    <t>30/mar</t>
-  </si>
-  <si>
-    <t>31/mar</t>
-  </si>
-  <si>
-    <t>01/abr</t>
-  </si>
-  <si>
-    <t>02/abr</t>
-  </si>
-  <si>
-    <t>03/abr</t>
-  </si>
-  <si>
-    <t>04/abr</t>
-  </si>
-  <si>
-    <t>05/abr</t>
-  </si>
-  <si>
-    <t>06/abr</t>
-  </si>
-  <si>
-    <t>07/abr</t>
-  </si>
-  <si>
-    <t>08/abr</t>
-  </si>
-  <si>
-    <t>09/abr</t>
-  </si>
-  <si>
-    <t>10/abr</t>
-  </si>
-  <si>
-    <t>11/abr</t>
-  </si>
-  <si>
-    <t>12/abr</t>
-  </si>
-  <si>
-    <t>13/abr</t>
-  </si>
-  <si>
-    <t>14/abr</t>
-  </si>
-  <si>
-    <t>15/abr</t>
-  </si>
-  <si>
-    <t>16/abr</t>
-  </si>
-  <si>
-    <t>17/abr</t>
-  </si>
-  <si>
-    <t>18/abr</t>
-  </si>
-  <si>
-    <t>19/abr</t>
-  </si>
-  <si>
-    <t>20/abr</t>
-  </si>
-  <si>
-    <t>21/abr</t>
-  </si>
-  <si>
-    <t>22/abr</t>
-  </si>
-  <si>
-    <t>23/abr</t>
-  </si>
-  <si>
-    <t>24/abr</t>
-  </si>
-  <si>
-    <t>25/abr</t>
-  </si>
-  <si>
-    <t>26/abr</t>
-  </si>
-  <si>
-    <t>27/abr</t>
-  </si>
-  <si>
-    <t>28/abr</t>
-  </si>
-  <si>
-    <t>29/abr</t>
-  </si>
-  <si>
-    <t>30/abr</t>
-  </si>
-  <si>
-    <t>01/mai</t>
-  </si>
-  <si>
-    <t>02/mai</t>
-  </si>
-  <si>
-    <t>03/mai</t>
-  </si>
-  <si>
-    <t>04/mai</t>
-  </si>
-  <si>
-    <t>05/mai</t>
-  </si>
-  <si>
-    <t>06/mai</t>
-  </si>
-  <si>
-    <t>07/mai</t>
-  </si>
-  <si>
-    <t>08/mai</t>
-  </si>
-  <si>
-    <t>09/mai</t>
-  </si>
-  <si>
-    <t>10/mai</t>
-  </si>
-  <si>
-    <t>11/mai</t>
-  </si>
-  <si>
-    <t>12/mai</t>
-  </si>
-  <si>
-    <t>13/mai</t>
-  </si>
-  <si>
-    <t>14/mai</t>
-  </si>
-  <si>
-    <t>15/mai</t>
-  </si>
-  <si>
-    <t>16/mai</t>
-  </si>
-  <si>
-    <t>17/mai</t>
-  </si>
-  <si>
-    <t>18/mai</t>
-  </si>
-  <si>
-    <t>19/mai</t>
-  </si>
-  <si>
-    <t>20/mai</t>
-  </si>
-  <si>
-    <t>21/mai</t>
-  </si>
-  <si>
-    <t>22/mai</t>
-  </si>
-  <si>
-    <t>23/mai</t>
-  </si>
-  <si>
-    <t>24/mai</t>
-  </si>
-  <si>
-    <t>25/mai</t>
-  </si>
-  <si>
-    <t>26/mai</t>
-  </si>
-  <si>
-    <t>27/mai</t>
-  </si>
-  <si>
-    <t>28/mai</t>
-  </si>
-  <si>
-    <t>29/mai</t>
-  </si>
-  <si>
-    <t>30/mai</t>
-  </si>
-  <si>
-    <t>31/mai</t>
-  </si>
-  <si>
-    <t>01/jun</t>
-  </si>
-  <si>
-    <t>02/jun</t>
-  </si>
-  <si>
-    <t>03/jun</t>
-  </si>
-  <si>
-    <t>04/jun</t>
-  </si>
-  <si>
-    <t>05/jun</t>
-  </si>
-  <si>
-    <t>06/jun</t>
-  </si>
-  <si>
-    <t>07/jun</t>
-  </si>
-  <si>
-    <t>08/jun</t>
-  </si>
-  <si>
-    <t>09/jun</t>
-  </si>
-  <si>
-    <t>10/jun</t>
-  </si>
-  <si>
-    <t>11/jun</t>
-  </si>
-  <si>
-    <t>12/jun</t>
-  </si>
-  <si>
-    <t>13/jun</t>
-  </si>
-  <si>
-    <t>14/jun</t>
-  </si>
-  <si>
-    <t>15/jun</t>
-  </si>
-  <si>
-    <t>16/jun</t>
-  </si>
-  <si>
-    <t>17/jun</t>
-  </si>
-  <si>
-    <t>18/jun</t>
-  </si>
-  <si>
-    <t>19/jun</t>
-  </si>
-  <si>
-    <t>20/jun</t>
-  </si>
-  <si>
-    <t>21/jun</t>
-  </si>
-  <si>
-    <t>22/jun</t>
-  </si>
-  <si>
-    <t>23/jun</t>
-  </si>
-  <si>
-    <t>24/jun</t>
-  </si>
-  <si>
-    <t>25/jun</t>
-  </si>
-  <si>
-    <t>26/jun</t>
-  </si>
-  <si>
-    <t>27/jun</t>
-  </si>
-  <si>
-    <t>28/jun</t>
-  </si>
-  <si>
-    <t>29/jun</t>
-  </si>
-  <si>
-    <t>30/jun</t>
-  </si>
-  <si>
-    <t>01/jul</t>
-  </si>
-  <si>
-    <t>02/jul</t>
-  </si>
-  <si>
-    <t>03/jul</t>
-  </si>
-  <si>
-    <t>04/jul</t>
-  </si>
-  <si>
-    <t>05/jul</t>
-  </si>
-  <si>
-    <t>06/jul</t>
-  </si>
-  <si>
-    <t>07/jul</t>
-  </si>
-  <si>
-    <t>08/jul</t>
-  </si>
-  <si>
-    <t>09/jul</t>
-  </si>
-  <si>
-    <t>10/jul</t>
-  </si>
-  <si>
-    <t>11/jul</t>
-  </si>
-  <si>
-    <t>12/jul</t>
-  </si>
-  <si>
-    <t>13/jul</t>
-  </si>
-  <si>
-    <t>14/jul</t>
-  </si>
-  <si>
-    <t>15/jul</t>
-  </si>
-  <si>
-    <t>16/jul</t>
-  </si>
-  <si>
-    <t>17/jul</t>
-  </si>
-  <si>
-    <t>18/jul</t>
-  </si>
-  <si>
-    <t>19/jul</t>
-  </si>
-  <si>
-    <t>20/jul</t>
-  </si>
-  <si>
-    <t>21/jul</t>
-  </si>
-  <si>
-    <t>22/jul</t>
-  </si>
-  <si>
-    <t>23/jul</t>
-  </si>
-  <si>
-    <t>24/jul</t>
-  </si>
-  <si>
-    <t>25/jul</t>
-  </si>
-  <si>
-    <t>26/jul</t>
-  </si>
-  <si>
-    <t>27/jul</t>
-  </si>
-  <si>
-    <t>28/jul</t>
-  </si>
-  <si>
-    <t>29/jul</t>
-  </si>
-  <si>
-    <t>30/jul</t>
-  </si>
-  <si>
-    <t>31/jul</t>
-  </si>
-  <si>
-    <t>01/ago</t>
-  </si>
-  <si>
-    <t>02/ago</t>
-  </si>
-  <si>
-    <t>03/ago</t>
-  </si>
-  <si>
-    <t>04/ago</t>
-  </si>
-  <si>
-    <t>05/ago</t>
-  </si>
-  <si>
-    <t>06/ago</t>
-  </si>
-  <si>
-    <t>07/ago</t>
-  </si>
-  <si>
-    <t>08/ago</t>
-  </si>
-  <si>
-    <t>09/ago</t>
-  </si>
-  <si>
-    <t>10/ago</t>
-  </si>
-  <si>
-    <t>11/ago</t>
-  </si>
-  <si>
-    <t>12/ago</t>
-  </si>
-  <si>
-    <t>13/ago</t>
-  </si>
-  <si>
-    <t>14/ago</t>
-  </si>
-  <si>
-    <t>15/ago</t>
-  </si>
-  <si>
-    <t>16/ago</t>
-  </si>
-  <si>
-    <t>17/ago</t>
-  </si>
-  <si>
-    <t>18/ago</t>
-  </si>
-  <si>
-    <t>19/ago</t>
-  </si>
-  <si>
-    <t>20/ago</t>
-  </si>
-  <si>
-    <t>21/ago</t>
-  </si>
-  <si>
-    <t>22/ago</t>
-  </si>
-  <si>
-    <t>23/ago</t>
-  </si>
-  <si>
-    <t>24/ago</t>
-  </si>
-  <si>
-    <t>25/ago</t>
-  </si>
-  <si>
-    <t>26/ago</t>
-  </si>
-  <si>
-    <t>27/ago</t>
-  </si>
-  <si>
-    <t>28/ago</t>
-  </si>
-  <si>
-    <t>29/ago</t>
-  </si>
-  <si>
-    <t>30/ago</t>
-  </si>
-  <si>
-    <t>31/ago</t>
-  </si>
-  <si>
-    <t>01/set</t>
-  </si>
-  <si>
-    <t>02/set</t>
-  </si>
-  <si>
-    <t>03/set</t>
-  </si>
-  <si>
-    <t>04/set</t>
-  </si>
-  <si>
-    <t>05/set</t>
-  </si>
-  <si>
-    <t>06/set</t>
-  </si>
-  <si>
-    <t>07/set</t>
-  </si>
-  <si>
-    <t>08/set</t>
-  </si>
-  <si>
-    <t>09/set</t>
-  </si>
-  <si>
-    <t>10/set</t>
-  </si>
-  <si>
-    <t>11/set</t>
-  </si>
-  <si>
-    <t>12/set</t>
-  </si>
-  <si>
-    <t>13/set</t>
-  </si>
-  <si>
-    <t>14/set</t>
-  </si>
-  <si>
-    <t>15/set</t>
-  </si>
-  <si>
-    <t>16/set</t>
-  </si>
-  <si>
-    <t>17/set</t>
-  </si>
-  <si>
-    <t>18/set</t>
-  </si>
-  <si>
-    <t>19/set</t>
-  </si>
-  <si>
-    <t>20/set</t>
-  </si>
-  <si>
-    <t>21/set</t>
-  </si>
-  <si>
-    <t>22/set</t>
-  </si>
-  <si>
-    <t>23/set</t>
-  </si>
-  <si>
-    <t>24/set</t>
-  </si>
-  <si>
-    <t>25/set</t>
-  </si>
-  <si>
-    <t>26/set</t>
-  </si>
-  <si>
-    <t>27/set</t>
-  </si>
-  <si>
-    <t>28/set</t>
-  </si>
-  <si>
-    <t>29/set</t>
-  </si>
-  <si>
-    <t>30/set</t>
-  </si>
-  <si>
-    <t>01/out</t>
-  </si>
-  <si>
-    <t>02/out</t>
-  </si>
-  <si>
-    <t>03/out</t>
-  </si>
-  <si>
-    <t>04/out</t>
-  </si>
-  <si>
-    <t>05/out</t>
-  </si>
-  <si>
-    <t>06/out</t>
-  </si>
-  <si>
-    <t>07/out</t>
-  </si>
-  <si>
-    <t>08/out</t>
-  </si>
-  <si>
-    <t>09/out</t>
-  </si>
-  <si>
-    <t>10/out</t>
-  </si>
-  <si>
-    <t>11/out</t>
-  </si>
-  <si>
-    <t>12/out</t>
-  </si>
-  <si>
-    <t>13/out</t>
-  </si>
-  <si>
-    <t>14/out</t>
-  </si>
-  <si>
-    <t>15/out</t>
-  </si>
-  <si>
-    <t>16/out</t>
-  </si>
-  <si>
-    <t>17/out</t>
-  </si>
-  <si>
-    <t>18/out</t>
-  </si>
-  <si>
-    <t>19/out</t>
-  </si>
-  <si>
-    <t>20/out</t>
-  </si>
-  <si>
-    <t>21/out</t>
-  </si>
-  <si>
-    <t>22/out</t>
-  </si>
-  <si>
-    <t>23/out</t>
-  </si>
-  <si>
-    <t>24/out</t>
-  </si>
-  <si>
-    <t>25/out</t>
-  </si>
-  <si>
-    <t>26/out</t>
-  </si>
-  <si>
-    <t>27/out</t>
-  </si>
-  <si>
-    <t>28/out</t>
-  </si>
-  <si>
-    <t>29/out</t>
-  </si>
-  <si>
-    <t>30/out</t>
-  </si>
-  <si>
-    <t>31/out</t>
-  </si>
-  <si>
-    <t>01/nov</t>
-  </si>
-  <si>
-    <t>02/nov</t>
-  </si>
-  <si>
-    <t>03/nov</t>
-  </si>
-  <si>
-    <t>04/nov</t>
-  </si>
-  <si>
-    <t>05/nov</t>
-  </si>
-  <si>
-    <t>06/nov</t>
-  </si>
-  <si>
-    <t>07/nov</t>
-  </si>
-  <si>
-    <t>08/nov</t>
-  </si>
-  <si>
-    <t>09/nov</t>
-  </si>
-  <si>
-    <t>10/nov</t>
-  </si>
-  <si>
-    <t>11/nov</t>
-  </si>
-  <si>
-    <t>12/nov</t>
-  </si>
-  <si>
-    <t>13/nov</t>
-  </si>
-  <si>
-    <t>14/nov</t>
-  </si>
-  <si>
-    <t>15/nov</t>
-  </si>
-  <si>
-    <t>16/nov</t>
-  </si>
-  <si>
-    <t>17/nov</t>
-  </si>
-  <si>
-    <t>18/nov</t>
-  </si>
-  <si>
-    <t>19/nov</t>
-  </si>
-  <si>
-    <t>20/nov</t>
-  </si>
-  <si>
-    <t>21/nov</t>
-  </si>
-  <si>
-    <t>22/nov</t>
-  </si>
-  <si>
-    <t>23/nov</t>
-  </si>
-  <si>
-    <t>24/nov</t>
-  </si>
-  <si>
-    <t>25/nov</t>
-  </si>
-  <si>
-    <t>26/nov</t>
-  </si>
-  <si>
-    <t>27/nov</t>
-  </si>
-  <si>
-    <t>28/nov</t>
-  </si>
-  <si>
-    <t>29/nov</t>
-  </si>
-  <si>
-    <t>30/nov</t>
-  </si>
-  <si>
-    <t>01/dez</t>
-  </si>
-  <si>
-    <t>02/dez</t>
-  </si>
-  <si>
-    <t>03/dez</t>
-  </si>
-  <si>
-    <t>04/dez</t>
-  </si>
-  <si>
-    <t>05/dez</t>
-  </si>
-  <si>
-    <t>06/dez</t>
-  </si>
-  <si>
-    <t>07/dez</t>
-  </si>
-  <si>
-    <t>08/dez</t>
-  </si>
-  <si>
-    <t>09/dez</t>
-  </si>
-  <si>
-    <t>10/dez</t>
-  </si>
-  <si>
-    <t>11/dez</t>
-  </si>
-  <si>
-    <t>12/dez</t>
-  </si>
-  <si>
-    <t>13/dez</t>
-  </si>
-  <si>
-    <t>14/dez</t>
-  </si>
-  <si>
-    <t>15/dez</t>
-  </si>
-  <si>
-    <t>16/dez</t>
-  </si>
-  <si>
-    <t>17/dez</t>
-  </si>
-  <si>
-    <t>18/dez</t>
-  </si>
-  <si>
-    <t>19/dez</t>
-  </si>
-  <si>
-    <t>20/dez</t>
-  </si>
-  <si>
-    <t>21/dez</t>
-  </si>
-  <si>
-    <t>22/dez</t>
-  </si>
-  <si>
-    <t>23/dez</t>
-  </si>
-  <si>
-    <t>24/dez</t>
-  </si>
-  <si>
-    <t>25/dez</t>
-  </si>
-  <si>
-    <t>26/dez</t>
-  </si>
-  <si>
-    <t>27/dez</t>
-  </si>
-  <si>
-    <t>28/dez</t>
-  </si>
-  <si>
-    <t>29/dez</t>
-  </si>
-  <si>
-    <t>30/dez</t>
-  </si>
-  <si>
-    <t>31/dez</t>
-  </si>
-  <si>
-    <t>01/jan</t>
-  </si>
-  <si>
-    <t>02/jan</t>
-  </si>
-  <si>
-    <t>03/jan</t>
-  </si>
-  <si>
-    <t>04/jan</t>
-  </si>
-  <si>
-    <t>05/jan</t>
-  </si>
-  <si>
-    <t>06/jan</t>
-  </si>
-  <si>
-    <t>07/jan</t>
-  </si>
-  <si>
-    <t>08/jan</t>
-  </si>
-  <si>
-    <t>09/jan</t>
-  </si>
-  <si>
-    <t>10/jan</t>
-  </si>
-  <si>
-    <t>11/jan</t>
-  </si>
-  <si>
-    <t>12/jan</t>
-  </si>
-  <si>
-    <t>13/jan</t>
-  </si>
-  <si>
-    <t>14/jan</t>
-  </si>
-  <si>
-    <t>15/jan</t>
-  </si>
-  <si>
-    <t>16/jan</t>
-  </si>
-  <si>
-    <t>17/jan</t>
-  </si>
-  <si>
-    <t>18/jan</t>
-  </si>
-  <si>
-    <t>19/jan</t>
-  </si>
-  <si>
-    <t>20/jan</t>
-  </si>
-  <si>
-    <t>21/jan</t>
-  </si>
-  <si>
-    <t>22/jan</t>
-  </si>
-  <si>
-    <t>23/jan</t>
-  </si>
-  <si>
-    <t>24/jan</t>
-  </si>
-  <si>
-    <t>25/jan</t>
-  </si>
-  <si>
-    <t>26/jan</t>
-  </si>
-  <si>
-    <t>27/jan</t>
-  </si>
-  <si>
-    <t>28/jan</t>
-  </si>
-  <si>
-    <t>29/jan</t>
-  </si>
-  <si>
-    <t>30/jan</t>
-  </si>
-  <si>
-    <t>31/jan</t>
-  </si>
-  <si>
-    <t>01/fev</t>
-  </si>
-  <si>
-    <t>02/fev</t>
-  </si>
-  <si>
-    <t>03/fev</t>
-  </si>
-  <si>
-    <t>04/fev</t>
-  </si>
-  <si>
-    <t>05/fev</t>
-  </si>
-  <si>
-    <t>06/fev</t>
-  </si>
-  <si>
-    <t>07/fev</t>
-  </si>
-  <si>
-    <t>08/fev</t>
-  </si>
-  <si>
-    <t>09/fev</t>
-  </si>
-  <si>
-    <t>10/fev</t>
-  </si>
-  <si>
-    <t>11/fev</t>
-  </si>
-  <si>
-    <t>12/fev</t>
-  </si>
-  <si>
-    <t>13/fev</t>
-  </si>
-  <si>
-    <t>14/fev</t>
-  </si>
-  <si>
-    <t>15/fev</t>
-  </si>
-  <si>
-    <t>16/fev</t>
-  </si>
-  <si>
-    <t>17/fev</t>
-  </si>
-  <si>
-    <t>18/fev</t>
-  </si>
-  <si>
-    <t>19/fev</t>
-  </si>
-  <si>
-    <t>20/fev</t>
-  </si>
-  <si>
-    <t>21/fev</t>
-  </si>
-  <si>
-    <t>22/fev</t>
-  </si>
-  <si>
-    <t>23/fev</t>
-  </si>
-  <si>
-    <t>24/fev</t>
-  </si>
-  <si>
-    <t>25/fev</t>
-  </si>
-  <si>
-    <t>26/fev</t>
-  </si>
-  <si>
-    <t>27/fev</t>
-  </si>
-  <si>
-    <t>28/fev</t>
-  </si>
-  <si>
-    <t>01/mar</t>
-  </si>
-  <si>
-    <t>02/mar</t>
-  </si>
-  <si>
-    <t>03/mar</t>
-  </si>
-  <si>
-    <t>04/mar</t>
-  </si>
-  <si>
-    <t>05/mar</t>
-  </si>
-  <si>
-    <t>06/mar</t>
-  </si>
-  <si>
-    <t>07/mar</t>
-  </si>
-  <si>
-    <t>08/mar</t>
-  </si>
-  <si>
-    <t>09/mar</t>
-  </si>
-  <si>
-    <t>10/mar</t>
-  </si>
-  <si>
-    <t>11/mar</t>
-  </si>
-  <si>
-    <t>12/mar</t>
-  </si>
-  <si>
-    <t>13/mar</t>
-  </si>
-  <si>
-    <t>14/mar</t>
-  </si>
-  <si>
-    <t>15/mar</t>
-  </si>
-  <si>
-    <t>16/mar</t>
-  </si>
-  <si>
-    <t>17/mar</t>
-  </si>
-  <si>
-    <t>18/mar</t>
-  </si>
-  <si>
-    <t>19/mar</t>
-  </si>
-  <si>
-    <t>20/mar</t>
-  </si>
-  <si>
-    <t>21/mar</t>
-  </si>
-  <si>
-    <t>22/mar</t>
+    <t>23/mar/2020</t>
+  </si>
+  <si>
+    <t>24/mar/2020</t>
+  </si>
+  <si>
+    <t>25/mar/2020</t>
+  </si>
+  <si>
+    <t>26/mar/2020</t>
+  </si>
+  <si>
+    <t>27/mar/2020</t>
+  </si>
+  <si>
+    <t>28/mar/2020</t>
+  </si>
+  <si>
+    <t>29/mar/2020</t>
+  </si>
+  <si>
+    <t>30/mar/2020</t>
+  </si>
+  <si>
+    <t>31/mar/2020</t>
+  </si>
+  <si>
+    <t>01/abr/2020</t>
+  </si>
+  <si>
+    <t>02/abr/2020</t>
+  </si>
+  <si>
+    <t>03/abr/2020</t>
+  </si>
+  <si>
+    <t>04/abr/2020</t>
+  </si>
+  <si>
+    <t>05/abr/2020</t>
+  </si>
+  <si>
+    <t>06/abr/2020</t>
+  </si>
+  <si>
+    <t>07/abr/2020</t>
+  </si>
+  <si>
+    <t>08/abr/2020</t>
+  </si>
+  <si>
+    <t>09/abr/2020</t>
+  </si>
+  <si>
+    <t>10/abr/2020</t>
+  </si>
+  <si>
+    <t>11/abr/2020</t>
+  </si>
+  <si>
+    <t>12/abr/2020</t>
+  </si>
+  <si>
+    <t>13/abr/2020</t>
+  </si>
+  <si>
+    <t>14/abr/2020</t>
+  </si>
+  <si>
+    <t>15/abr/2020</t>
+  </si>
+  <si>
+    <t>16/abr/2020</t>
+  </si>
+  <si>
+    <t>17/abr/2020</t>
+  </si>
+  <si>
+    <t>18/abr/2020</t>
+  </si>
+  <si>
+    <t>19/abr/2020</t>
+  </si>
+  <si>
+    <t>20/abr/2020</t>
+  </si>
+  <si>
+    <t>21/abr/2020</t>
+  </si>
+  <si>
+    <t>22/abr/2020</t>
+  </si>
+  <si>
+    <t>23/abr/2020</t>
+  </si>
+  <si>
+    <t>24/abr/2020</t>
+  </si>
+  <si>
+    <t>25/abr/2020</t>
+  </si>
+  <si>
+    <t>26/abr/2020</t>
+  </si>
+  <si>
+    <t>27/abr/2020</t>
+  </si>
+  <si>
+    <t>28/abr/2020</t>
+  </si>
+  <si>
+    <t>29/abr/2020</t>
+  </si>
+  <si>
+    <t>30/abr/2020</t>
+  </si>
+  <si>
+    <t>01/mai/2020</t>
+  </si>
+  <si>
+    <t>02/mai/2020</t>
+  </si>
+  <si>
+    <t>03/mai/2020</t>
+  </si>
+  <si>
+    <t>04/mai/2020</t>
+  </si>
+  <si>
+    <t>05/mai/2020</t>
+  </si>
+  <si>
+    <t>06/mai/2020</t>
+  </si>
+  <si>
+    <t>07/mai/2020</t>
+  </si>
+  <si>
+    <t>08/mai/2020</t>
+  </si>
+  <si>
+    <t>09/mai/2020</t>
+  </si>
+  <si>
+    <t>10/mai/2020</t>
+  </si>
+  <si>
+    <t>11/mai/2020</t>
+  </si>
+  <si>
+    <t>12/mai/2020</t>
+  </si>
+  <si>
+    <t>13/mai/2020</t>
+  </si>
+  <si>
+    <t>14/mai/2020</t>
+  </si>
+  <si>
+    <t>15/mai/2020</t>
+  </si>
+  <si>
+    <t>16/mai/2020</t>
+  </si>
+  <si>
+    <t>17/mai/2020</t>
+  </si>
+  <si>
+    <t>18/mai/2020</t>
+  </si>
+  <si>
+    <t>19/mai/2020</t>
+  </si>
+  <si>
+    <t>20/mai/2020</t>
+  </si>
+  <si>
+    <t>21/mai/2020</t>
+  </si>
+  <si>
+    <t>22/mai/2020</t>
+  </si>
+  <si>
+    <t>23/mai/2020</t>
+  </si>
+  <si>
+    <t>24/mai/2020</t>
+  </si>
+  <si>
+    <t>25/mai/2020</t>
+  </si>
+  <si>
+    <t>26/mai/2020</t>
+  </si>
+  <si>
+    <t>27/mai/2020</t>
+  </si>
+  <si>
+    <t>28/mai/2020</t>
+  </si>
+  <si>
+    <t>29/mai/2020</t>
+  </si>
+  <si>
+    <t>30/mai/2020</t>
+  </si>
+  <si>
+    <t>31/mai/2020</t>
+  </si>
+  <si>
+    <t>01/jun/2020</t>
+  </si>
+  <si>
+    <t>02/jun/2020</t>
+  </si>
+  <si>
+    <t>03/jun/2020</t>
+  </si>
+  <si>
+    <t>04/jun/2020</t>
+  </si>
+  <si>
+    <t>05/jun/2020</t>
+  </si>
+  <si>
+    <t>06/jun/2020</t>
+  </si>
+  <si>
+    <t>07/jun/2020</t>
+  </si>
+  <si>
+    <t>08/jun/2020</t>
+  </si>
+  <si>
+    <t>09/jun/2020</t>
+  </si>
+  <si>
+    <t>10/jun/2020</t>
+  </si>
+  <si>
+    <t>11/jun/2020</t>
+  </si>
+  <si>
+    <t>12/jun/2020</t>
+  </si>
+  <si>
+    <t>13/jun/2020</t>
+  </si>
+  <si>
+    <t>14/jun/2020</t>
+  </si>
+  <si>
+    <t>15/jun/2020</t>
+  </si>
+  <si>
+    <t>16/jun/2020</t>
+  </si>
+  <si>
+    <t>17/jun/2020</t>
+  </si>
+  <si>
+    <t>18/jun/2020</t>
+  </si>
+  <si>
+    <t>19/jun/2020</t>
+  </si>
+  <si>
+    <t>20/jun/2020</t>
+  </si>
+  <si>
+    <t>21/jun/2020</t>
+  </si>
+  <si>
+    <t>22/jun/2020</t>
+  </si>
+  <si>
+    <t>23/jun/2020</t>
+  </si>
+  <si>
+    <t>24/jun/2020</t>
+  </si>
+  <si>
+    <t>25/jun/2020</t>
+  </si>
+  <si>
+    <t>26/jun/2020</t>
+  </si>
+  <si>
+    <t>27/jun/2020</t>
+  </si>
+  <si>
+    <t>28/jun/2020</t>
+  </si>
+  <si>
+    <t>29/jun/2020</t>
+  </si>
+  <si>
+    <t>30/jun/2020</t>
+  </si>
+  <si>
+    <t>01/jul/2020</t>
+  </si>
+  <si>
+    <t>02/jul/2020</t>
+  </si>
+  <si>
+    <t>03/jul/2020</t>
+  </si>
+  <si>
+    <t>04/jul/2020</t>
+  </si>
+  <si>
+    <t>05/jul/2020</t>
+  </si>
+  <si>
+    <t>06/jul/2020</t>
+  </si>
+  <si>
+    <t>07/jul/2020</t>
+  </si>
+  <si>
+    <t>08/jul/2020</t>
+  </si>
+  <si>
+    <t>09/jul/2020</t>
+  </si>
+  <si>
+    <t>10/jul/2020</t>
+  </si>
+  <si>
+    <t>11/jul/2020</t>
+  </si>
+  <si>
+    <t>12/jul/2020</t>
+  </si>
+  <si>
+    <t>13/jul/2020</t>
+  </si>
+  <si>
+    <t>14/jul/2020</t>
+  </si>
+  <si>
+    <t>15/jul/2020</t>
+  </si>
+  <si>
+    <t>16/jul/2020</t>
+  </si>
+  <si>
+    <t>17/jul/2020</t>
+  </si>
+  <si>
+    <t>18/jul/2020</t>
+  </si>
+  <si>
+    <t>19/jul/2020</t>
+  </si>
+  <si>
+    <t>20/jul/2020</t>
+  </si>
+  <si>
+    <t>21/jul/2020</t>
+  </si>
+  <si>
+    <t>22/jul/2020</t>
+  </si>
+  <si>
+    <t>23/jul/2020</t>
+  </si>
+  <si>
+    <t>24/jul/2020</t>
+  </si>
+  <si>
+    <t>25/jul/2020</t>
+  </si>
+  <si>
+    <t>26/jul/2020</t>
+  </si>
+  <si>
+    <t>27/jul/2020</t>
+  </si>
+  <si>
+    <t>28/jul/2020</t>
+  </si>
+  <si>
+    <t>29/jul/2020</t>
+  </si>
+  <si>
+    <t>30/jul/2020</t>
+  </si>
+  <si>
+    <t>31/jul/2020</t>
+  </si>
+  <si>
+    <t>01/ago/2020</t>
+  </si>
+  <si>
+    <t>02/ago/2020</t>
+  </si>
+  <si>
+    <t>03/ago/2020</t>
+  </si>
+  <si>
+    <t>04/ago/2020</t>
+  </si>
+  <si>
+    <t>05/ago/2020</t>
+  </si>
+  <si>
+    <t>06/ago/2020</t>
+  </si>
+  <si>
+    <t>07/ago/2020</t>
+  </si>
+  <si>
+    <t>08/ago/2020</t>
+  </si>
+  <si>
+    <t>09/ago/2020</t>
+  </si>
+  <si>
+    <t>10/ago/2020</t>
+  </si>
+  <si>
+    <t>11/ago/2020</t>
+  </si>
+  <si>
+    <t>12/ago/2020</t>
+  </si>
+  <si>
+    <t>13/ago/2020</t>
+  </si>
+  <si>
+    <t>14/ago/2020</t>
+  </si>
+  <si>
+    <t>15/ago/2020</t>
+  </si>
+  <si>
+    <t>16/ago/2020</t>
+  </si>
+  <si>
+    <t>17/ago/2020</t>
+  </si>
+  <si>
+    <t>18/ago/2020</t>
+  </si>
+  <si>
+    <t>19/ago/2020</t>
+  </si>
+  <si>
+    <t>20/ago/2020</t>
+  </si>
+  <si>
+    <t>21/ago/2020</t>
+  </si>
+  <si>
+    <t>22/ago/2020</t>
+  </si>
+  <si>
+    <t>23/ago/2020</t>
+  </si>
+  <si>
+    <t>24/ago/2020</t>
+  </si>
+  <si>
+    <t>25/ago/2020</t>
+  </si>
+  <si>
+    <t>26/ago/2020</t>
+  </si>
+  <si>
+    <t>27/ago/2020</t>
+  </si>
+  <si>
+    <t>28/ago/2020</t>
+  </si>
+  <si>
+    <t>29/ago/2020</t>
+  </si>
+  <si>
+    <t>30/ago/2020</t>
+  </si>
+  <si>
+    <t>31/ago/2020</t>
+  </si>
+  <si>
+    <t>01/set/2020</t>
+  </si>
+  <si>
+    <t>02/set/2020</t>
+  </si>
+  <si>
+    <t>03/set/2020</t>
+  </si>
+  <si>
+    <t>04/set/2020</t>
+  </si>
+  <si>
+    <t>05/set/2020</t>
+  </si>
+  <si>
+    <t>06/set/2020</t>
+  </si>
+  <si>
+    <t>07/set/2020</t>
+  </si>
+  <si>
+    <t>08/set/2020</t>
+  </si>
+  <si>
+    <t>09/set/2020</t>
+  </si>
+  <si>
+    <t>10/set/2020</t>
+  </si>
+  <si>
+    <t>11/set/2020</t>
+  </si>
+  <si>
+    <t>12/set/2020</t>
+  </si>
+  <si>
+    <t>13/set/2020</t>
+  </si>
+  <si>
+    <t>14/set/2020</t>
+  </si>
+  <si>
+    <t>15/set/2020</t>
+  </si>
+  <si>
+    <t>16/set/2020</t>
+  </si>
+  <si>
+    <t>17/set/2020</t>
+  </si>
+  <si>
+    <t>18/set/2020</t>
+  </si>
+  <si>
+    <t>19/set/2020</t>
+  </si>
+  <si>
+    <t>20/set/2020</t>
+  </si>
+  <si>
+    <t>21/set/2020</t>
+  </si>
+  <si>
+    <t>22/set/2020</t>
+  </si>
+  <si>
+    <t>23/set/2020</t>
+  </si>
+  <si>
+    <t>24/set/2020</t>
+  </si>
+  <si>
+    <t>25/set/2020</t>
+  </si>
+  <si>
+    <t>26/set/2020</t>
+  </si>
+  <si>
+    <t>27/set/2020</t>
+  </si>
+  <si>
+    <t>28/set/2020</t>
+  </si>
+  <si>
+    <t>29/set/2020</t>
+  </si>
+  <si>
+    <t>30/set/2020</t>
+  </si>
+  <si>
+    <t>01/out/2020</t>
+  </si>
+  <si>
+    <t>02/out/2020</t>
+  </si>
+  <si>
+    <t>03/out/2020</t>
+  </si>
+  <si>
+    <t>04/out/2020</t>
+  </si>
+  <si>
+    <t>05/out/2020</t>
+  </si>
+  <si>
+    <t>06/out/2020</t>
+  </si>
+  <si>
+    <t>07/out/2020</t>
+  </si>
+  <si>
+    <t>08/out/2020</t>
+  </si>
+  <si>
+    <t>09/out/2020</t>
+  </si>
+  <si>
+    <t>10/out/2020</t>
+  </si>
+  <si>
+    <t>11/out/2020</t>
+  </si>
+  <si>
+    <t>12/out/2020</t>
+  </si>
+  <si>
+    <t>13/out/2020</t>
+  </si>
+  <si>
+    <t>14/out/2020</t>
+  </si>
+  <si>
+    <t>15/out/2020</t>
+  </si>
+  <si>
+    <t>16/out/2020</t>
+  </si>
+  <si>
+    <t>17/out/2020</t>
+  </si>
+  <si>
+    <t>18/out/2020</t>
+  </si>
+  <si>
+    <t>19/out/2020</t>
+  </si>
+  <si>
+    <t>20/out/2020</t>
+  </si>
+  <si>
+    <t>21/out/2020</t>
+  </si>
+  <si>
+    <t>22/out/2020</t>
+  </si>
+  <si>
+    <t>23/out/2020</t>
+  </si>
+  <si>
+    <t>24/out/2020</t>
+  </si>
+  <si>
+    <t>25/out/2020</t>
+  </si>
+  <si>
+    <t>26/out/2020</t>
+  </si>
+  <si>
+    <t>27/out/2020</t>
+  </si>
+  <si>
+    <t>28/out/2020</t>
+  </si>
+  <si>
+    <t>29/out/2020</t>
+  </si>
+  <si>
+    <t>30/out/2020</t>
+  </si>
+  <si>
+    <t>31/out/2020</t>
+  </si>
+  <si>
+    <t>01/nov/2020</t>
+  </si>
+  <si>
+    <t>02/nov/2020</t>
+  </si>
+  <si>
+    <t>03/nov/2020</t>
+  </si>
+  <si>
+    <t>04/nov/2020</t>
+  </si>
+  <si>
+    <t>05/nov/2020</t>
+  </si>
+  <si>
+    <t>06/nov/2020</t>
+  </si>
+  <si>
+    <t>07/nov/2020</t>
+  </si>
+  <si>
+    <t>08/nov/2020</t>
+  </si>
+  <si>
+    <t>09/nov/2020</t>
+  </si>
+  <si>
+    <t>10/nov/2020</t>
+  </si>
+  <si>
+    <t>11/nov/2020</t>
+  </si>
+  <si>
+    <t>12/nov/2020</t>
+  </si>
+  <si>
+    <t>13/nov/2020</t>
+  </si>
+  <si>
+    <t>14/nov/2020</t>
+  </si>
+  <si>
+    <t>15/nov/2020</t>
+  </si>
+  <si>
+    <t>16/nov/2020</t>
+  </si>
+  <si>
+    <t>17/nov/2020</t>
+  </si>
+  <si>
+    <t>18/nov/2020</t>
+  </si>
+  <si>
+    <t>19/nov/2020</t>
+  </si>
+  <si>
+    <t>20/nov/2020</t>
+  </si>
+  <si>
+    <t>21/nov/2020</t>
+  </si>
+  <si>
+    <t>22/nov/2020</t>
+  </si>
+  <si>
+    <t>23/nov/2020</t>
+  </si>
+  <si>
+    <t>24/nov/2020</t>
+  </si>
+  <si>
+    <t>25/nov/2020</t>
+  </si>
+  <si>
+    <t>26/nov/2020</t>
+  </si>
+  <si>
+    <t>27/nov/2020</t>
+  </si>
+  <si>
+    <t>28/nov/2020</t>
+  </si>
+  <si>
+    <t>29/nov/2020</t>
+  </si>
+  <si>
+    <t>30/nov/2020</t>
+  </si>
+  <si>
+    <t>01/dez/2020</t>
+  </si>
+  <si>
+    <t>02/dez/2020</t>
+  </si>
+  <si>
+    <t>03/dez/2020</t>
+  </si>
+  <si>
+    <t>04/dez/2020</t>
+  </si>
+  <si>
+    <t>05/dez/2020</t>
+  </si>
+  <si>
+    <t>06/dez/2020</t>
+  </si>
+  <si>
+    <t>07/dez/2020</t>
+  </si>
+  <si>
+    <t>08/dez/2020</t>
+  </si>
+  <si>
+    <t>09/dez/2020</t>
+  </si>
+  <si>
+    <t>10/dez/2020</t>
+  </si>
+  <si>
+    <t>11/dez/2020</t>
+  </si>
+  <si>
+    <t>12/dez/2020</t>
+  </si>
+  <si>
+    <t>13/dez/2020</t>
+  </si>
+  <si>
+    <t>14/dez/2020</t>
+  </si>
+  <si>
+    <t>15/dez/2020</t>
+  </si>
+  <si>
+    <t>16/dez/2020</t>
+  </si>
+  <si>
+    <t>17/dez/2020</t>
+  </si>
+  <si>
+    <t>18/dez/2020</t>
+  </si>
+  <si>
+    <t>19/dez/2020</t>
+  </si>
+  <si>
+    <t>20/dez/2020</t>
+  </si>
+  <si>
+    <t>21/dez/2020</t>
+  </si>
+  <si>
+    <t>22/dez/2020</t>
+  </si>
+  <si>
+    <t>23/dez/2020</t>
+  </si>
+  <si>
+    <t>24/dez/2020</t>
+  </si>
+  <si>
+    <t>25/dez/2020</t>
+  </si>
+  <si>
+    <t>26/dez/2020</t>
+  </si>
+  <si>
+    <t>27/dez/2020</t>
+  </si>
+  <si>
+    <t>28/dez/2020</t>
+  </si>
+  <si>
+    <t>29/dez/2020</t>
+  </si>
+  <si>
+    <t>30/dez/2020</t>
+  </si>
+  <si>
+    <t>31/dez/2020</t>
+  </si>
+  <si>
+    <t>01/jan/2021</t>
+  </si>
+  <si>
+    <t>02/jan/2021</t>
+  </si>
+  <si>
+    <t>03/jan/2021</t>
+  </si>
+  <si>
+    <t>04/jan/2021</t>
+  </si>
+  <si>
+    <t>05/jan/2021</t>
+  </si>
+  <si>
+    <t>06/jan/2021</t>
+  </si>
+  <si>
+    <t>07/jan/2021</t>
+  </si>
+  <si>
+    <t>08/jan/2021</t>
+  </si>
+  <si>
+    <t>09/jan/2021</t>
+  </si>
+  <si>
+    <t>10/jan/2021</t>
+  </si>
+  <si>
+    <t>11/jan/2021</t>
+  </si>
+  <si>
+    <t>12/jan/2021</t>
+  </si>
+  <si>
+    <t>13/jan/2021</t>
+  </si>
+  <si>
+    <t>14/jan/2021</t>
+  </si>
+  <si>
+    <t>15/jan/2021</t>
+  </si>
+  <si>
+    <t>16/jan/2021</t>
+  </si>
+  <si>
+    <t>17/jan/2021</t>
+  </si>
+  <si>
+    <t>18/jan/2021</t>
+  </si>
+  <si>
+    <t>19/jan/2021</t>
+  </si>
+  <si>
+    <t>20/jan/2021</t>
+  </si>
+  <si>
+    <t>21/jan/2021</t>
+  </si>
+  <si>
+    <t>22/jan/2021</t>
+  </si>
+  <si>
+    <t>23/jan/2021</t>
+  </si>
+  <si>
+    <t>24/jan/2021</t>
+  </si>
+  <si>
+    <t>25/jan/2021</t>
+  </si>
+  <si>
+    <t>26/jan/2021</t>
+  </si>
+  <si>
+    <t>27/jan/2021</t>
+  </si>
+  <si>
+    <t>28/jan/2021</t>
+  </si>
+  <si>
+    <t>29/jan/2021</t>
+  </si>
+  <si>
+    <t>30/jan/2021</t>
+  </si>
+  <si>
+    <t>31/jan/2021</t>
+  </si>
+  <si>
+    <t>01/fev/2021</t>
+  </si>
+  <si>
+    <t>02/fev/2021</t>
+  </si>
+  <si>
+    <t>03/fev/2021</t>
+  </si>
+  <si>
+    <t>04/fev/2021</t>
+  </si>
+  <si>
+    <t>05/fev/2021</t>
+  </si>
+  <si>
+    <t>06/fev/2021</t>
+  </si>
+  <si>
+    <t>07/fev/2021</t>
+  </si>
+  <si>
+    <t>08/fev/2021</t>
+  </si>
+  <si>
+    <t>09/fev/2021</t>
+  </si>
+  <si>
+    <t>10/fev/2021</t>
+  </si>
+  <si>
+    <t>11/fev/2021</t>
+  </si>
+  <si>
+    <t>12/fev/2021</t>
+  </si>
+  <si>
+    <t>13/fev/2021</t>
+  </si>
+  <si>
+    <t>14/fev/2021</t>
+  </si>
+  <si>
+    <t>15/fev/2021</t>
+  </si>
+  <si>
+    <t>16/fev/2021</t>
+  </si>
+  <si>
+    <t>17/fev/2021</t>
+  </si>
+  <si>
+    <t>18/fev/2021</t>
+  </si>
+  <si>
+    <t>19/fev/2021</t>
+  </si>
+  <si>
+    <t>20/fev/2021</t>
+  </si>
+  <si>
+    <t>21/fev/2021</t>
+  </si>
+  <si>
+    <t>22/fev/2021</t>
+  </si>
+  <si>
+    <t>23/fev/2021</t>
+  </si>
+  <si>
+    <t>24/fev/2021</t>
+  </si>
+  <si>
+    <t>25/fev/2021</t>
+  </si>
+  <si>
+    <t>26/fev/2021</t>
+  </si>
+  <si>
+    <t>27/fev/2021</t>
+  </si>
+  <si>
+    <t>28/fev/2021</t>
+  </si>
+  <si>
+    <t>01/mar/2021</t>
+  </si>
+  <si>
+    <t>02/mar/2021</t>
+  </si>
+  <si>
+    <t>03/mar/2021</t>
+  </si>
+  <si>
+    <t>04/mar/2021</t>
+  </si>
+  <si>
+    <t>05/mar/2021</t>
+  </si>
+  <si>
+    <t>06/mar/2021</t>
+  </si>
+  <si>
+    <t>07/mar/2021</t>
+  </si>
+  <si>
+    <t>08/mar/2021</t>
+  </si>
+  <si>
+    <t>09/mar/2021</t>
+  </si>
+  <si>
+    <t>10/mar/2021</t>
+  </si>
+  <si>
+    <t>11/mar/2021</t>
+  </si>
+  <si>
+    <t>12/mar/2021</t>
+  </si>
+  <si>
+    <t>13/mar/2021</t>
+  </si>
+  <si>
+    <t>14/mar/2021</t>
+  </si>
+  <si>
+    <t>15/mar/2021</t>
+  </si>
+  <si>
+    <t>16/mar/2021</t>
+  </si>
+  <si>
+    <t>17/mar/2021</t>
+  </si>
+  <si>
+    <t>18/mar/2021</t>
+  </si>
+  <si>
+    <t>19/mar/2021</t>
+  </si>
+  <si>
+    <t>20/mar/2021</t>
+  </si>
+  <si>
+    <t>21/mar/2021</t>
+  </si>
+  <si>
+    <t>22/mar/2021</t>
+  </si>
+  <si>
+    <t>23/mar/2021</t>
+  </si>
+  <si>
+    <t>24/mar/2021</t>
+  </si>
+  <si>
+    <t>25/mar/2021</t>
+  </si>
+  <si>
+    <t>26/mar/2021</t>
+  </si>
+  <si>
+    <t>27/mar/2021</t>
+  </si>
+  <si>
+    <t>28/mar/2021</t>
+  </si>
+  <si>
+    <t>29/mar/2021</t>
+  </si>
+  <si>
+    <t>30/mar/2021</t>
+  </si>
+  <si>
+    <t>31/mar/2021</t>
+  </si>
+  <si>
+    <t>01/abr/2021</t>
+  </si>
+  <si>
+    <t>02/abr/2021</t>
+  </si>
+  <si>
+    <t>03/abr/2021</t>
+  </si>
+  <si>
+    <t>04/abr/2021</t>
+  </si>
+  <si>
+    <t>05/abr/2021</t>
+  </si>
+  <si>
+    <t>06/abr/2021</t>
+  </si>
+  <si>
+    <t>07/abr/2021</t>
+  </si>
+  <si>
+    <t>08/abr/2021</t>
+  </si>
+  <si>
+    <t>09/abr/2021</t>
+  </si>
+  <si>
+    <t>10/abr/2021</t>
+  </si>
+  <si>
+    <t>11/abr/2021</t>
+  </si>
+  <si>
+    <t>12/abr/2021</t>
+  </si>
+  <si>
+    <t>13/abr/2021</t>
+  </si>
+  <si>
+    <t>14/abr/2021</t>
+  </si>
+  <si>
+    <t>15/abr/2021</t>
+  </si>
+  <si>
+    <t>16/abr/2021</t>
+  </si>
+  <si>
+    <t>17/abr/2021</t>
+  </si>
+  <si>
+    <t>18/abr/2021</t>
+  </si>
+  <si>
+    <t>19/abr/2021</t>
+  </si>
+  <si>
+    <t>20/abr/2021</t>
+  </si>
+  <si>
+    <t>21/abr/2021</t>
+  </si>
+  <si>
+    <t>22/abr/2021</t>
+  </si>
+  <si>
+    <t>23/abr/2021</t>
+  </si>
+  <si>
+    <t>24/abr/2021</t>
+  </si>
+  <si>
+    <t>25/abr/2021</t>
+  </si>
+  <si>
+    <t>26/abr/2021</t>
+  </si>
+  <si>
+    <t>27/abr/2021</t>
+  </si>
+  <si>
+    <t>28/abr/2021</t>
+  </si>
+  <si>
+    <t>29/abr/2021</t>
+  </si>
+  <si>
+    <t>30/abr/2021</t>
+  </si>
+  <si>
+    <t>01/mai/2021</t>
+  </si>
+  <si>
+    <t>02/mai/2021</t>
+  </si>
+  <si>
+    <t>03/mai/2021</t>
+  </si>
+  <si>
+    <t>04/mai/2021</t>
+  </si>
+  <si>
+    <t>05/mai/2021</t>
+  </si>
+  <si>
+    <t>06/mai/2021</t>
+  </si>
+  <si>
+    <t>07/mai/2021</t>
+  </si>
+  <si>
+    <t>08/mai/2021</t>
+  </si>
+  <si>
+    <t>09/mai/2021</t>
+  </si>
+  <si>
+    <t>10/mai/2021</t>
+  </si>
+  <si>
+    <t>11/mai/2021</t>
+  </si>
+  <si>
+    <t>12/mai/2021</t>
+  </si>
+  <si>
+    <t>13/mai/2021</t>
+  </si>
+  <si>
+    <t>14/mai/2021</t>
+  </si>
+  <si>
+    <t>15/mai/2021</t>
+  </si>
+  <si>
+    <t>16/mai/2021</t>
+  </si>
+  <si>
+    <t>17/mai/2021</t>
+  </si>
+  <si>
+    <t>18/mai/2021</t>
+  </si>
+  <si>
+    <t>19/mai/2021</t>
+  </si>
+  <si>
+    <t>20/mai/2021</t>
+  </si>
+  <si>
+    <t>21/mai/2021</t>
+  </si>
+  <si>
+    <t>22/mai/2021</t>
+  </si>
+  <si>
+    <t>23/mai/2021</t>
+  </si>
+  <si>
+    <t>24/mai/2021</t>
+  </si>
+  <si>
+    <t>25/mai/2021</t>
+  </si>
+  <si>
+    <t>26/mai/2021</t>
+  </si>
+  <si>
+    <t>27/mai/2021</t>
+  </si>
+  <si>
+    <t>28/mai/2021</t>
+  </si>
+  <si>
+    <t>29/mai/2021</t>
+  </si>
+  <si>
+    <t>30/mai/2021</t>
+  </si>
+  <si>
+    <t>31/mai/2021</t>
+  </si>
+  <si>
+    <t>01/jun/2021</t>
+  </si>
+  <si>
+    <t>02/jun/2021</t>
+  </si>
+  <si>
+    <t>03/jun/2021</t>
+  </si>
+  <si>
+    <t>04/jun/2021</t>
+  </si>
+  <si>
+    <t>05/jun/2021</t>
+  </si>
+  <si>
+    <t>06/jun/2021</t>
+  </si>
+  <si>
+    <t>07/jun/2021</t>
+  </si>
+  <si>
+    <t>08/jun/2021</t>
+  </si>
+  <si>
+    <t>09/jun/2021</t>
+  </si>
+  <si>
+    <t>10/jun/2021</t>
+  </si>
+  <si>
+    <t>11/jun/2021</t>
+  </si>
+  <si>
+    <t>12/jun/2021</t>
+  </si>
+  <si>
+    <t>13/jun/2021</t>
+  </si>
+  <si>
+    <t>14/jun/2021</t>
+  </si>
+  <si>
+    <t>15/jun/2021</t>
+  </si>
+  <si>
+    <t>16/jun/2021</t>
+  </si>
+  <si>
+    <t>17/jun/2021</t>
+  </si>
+  <si>
+    <t>18/jun/2021</t>
+  </si>
+  <si>
+    <t>19/jun/2021</t>
+  </si>
+  <si>
+    <t>20/jun/2021</t>
+  </si>
+  <si>
+    <t>21/jun/2021</t>
+  </si>
+  <si>
+    <t>22/jun/2021</t>
+  </si>
+  <si>
+    <t>23/jun/2021</t>
+  </si>
+  <si>
+    <t>24/jun/2021</t>
+  </si>
+  <si>
+    <t>25/jun/2021</t>
+  </si>
+  <si>
+    <t>26/jun/2021</t>
+  </si>
+  <si>
+    <t>27/jun/2021</t>
+  </si>
+  <si>
+    <t>28/jun/2021</t>
   </si>
 </sst>
 </file>
@@ -1484,7 +1778,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G452"/>
+  <dimension ref="A1:G464"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -9907,7 +10201,7 @@
     </row>
     <row r="367" spans="1:7">
       <c r="A367" s="1" t="s">
-        <v>6</v>
+        <v>371</v>
       </c>
       <c r="B367">
         <v>11200</v>
@@ -9925,12 +10219,12 @@
         <v>218162</v>
       </c>
       <c r="G367" t="s">
-        <v>6</v>
+        <v>371</v>
       </c>
     </row>
     <row r="368" spans="1:7">
       <c r="A368" s="1" t="s">
-        <v>7</v>
+        <v>372</v>
       </c>
       <c r="B368">
         <v>11311</v>
@@ -9948,12 +10242,12 @@
         <v>218162</v>
       </c>
       <c r="G368" t="s">
-        <v>7</v>
+        <v>372</v>
       </c>
     </row>
     <row r="369" spans="1:7">
       <c r="A369" s="1" t="s">
-        <v>8</v>
+        <v>373</v>
       </c>
       <c r="B369">
         <v>11425</v>
@@ -9971,12 +10265,12 @@
         <v>218162</v>
       </c>
       <c r="G369" t="s">
-        <v>8</v>
+        <v>373</v>
       </c>
     </row>
     <row r="370" spans="1:7">
       <c r="A370" s="1" t="s">
-        <v>9</v>
+        <v>374</v>
       </c>
       <c r="B370">
         <v>11496</v>
@@ -9994,12 +10288,12 @@
         <v>218162</v>
       </c>
       <c r="G370" t="s">
-        <v>9</v>
+        <v>374</v>
       </c>
     </row>
     <row r="371" spans="1:7">
       <c r="A371" s="1" t="s">
-        <v>10</v>
+        <v>375</v>
       </c>
       <c r="B371">
         <v>11584</v>
@@ -10017,12 +10311,12 @@
         <v>218162</v>
       </c>
       <c r="G371" t="s">
-        <v>10</v>
+        <v>375</v>
       </c>
     </row>
     <row r="372" spans="1:7">
       <c r="A372" s="1" t="s">
-        <v>11</v>
+        <v>376</v>
       </c>
       <c r="B372">
         <v>11642</v>
@@ -10040,12 +10334,12 @@
         <v>218162</v>
       </c>
       <c r="G372" t="s">
-        <v>11</v>
+        <v>376</v>
       </c>
     </row>
     <row r="373" spans="1:7">
       <c r="A373" s="1" t="s">
-        <v>12</v>
+        <v>377</v>
       </c>
       <c r="B373">
         <v>11659</v>
@@ -10063,12 +10357,12 @@
         <v>218162</v>
       </c>
       <c r="G373" t="s">
-        <v>12</v>
+        <v>377</v>
       </c>
     </row>
     <row r="374" spans="1:7">
       <c r="A374" s="1" t="s">
-        <v>13</v>
+        <v>378</v>
       </c>
       <c r="B374">
         <v>11697</v>
@@ -10086,12 +10380,12 @@
         <v>218162</v>
       </c>
       <c r="G374" t="s">
-        <v>13</v>
+        <v>378</v>
       </c>
     </row>
     <row r="375" spans="1:7">
       <c r="A375" s="1" t="s">
-        <v>14</v>
+        <v>379</v>
       </c>
       <c r="B375">
         <v>11809</v>
@@ -10109,12 +10403,12 @@
         <v>218162</v>
       </c>
       <c r="G375" t="s">
-        <v>14</v>
+        <v>379</v>
       </c>
     </row>
     <row r="376" spans="1:7">
       <c r="A376" s="1" t="s">
-        <v>15</v>
+        <v>380</v>
       </c>
       <c r="B376">
         <v>11904</v>
@@ -10132,12 +10426,12 @@
         <v>218162</v>
       </c>
       <c r="G376" t="s">
-        <v>15</v>
+        <v>380</v>
       </c>
     </row>
     <row r="377" spans="1:7">
       <c r="A377" s="1" t="s">
-        <v>16</v>
+        <v>381</v>
       </c>
       <c r="B377">
         <v>12009</v>
@@ -10155,12 +10449,12 @@
         <v>218162</v>
       </c>
       <c r="G377" t="s">
-        <v>16</v>
+        <v>381</v>
       </c>
     </row>
     <row r="378" spans="1:7">
       <c r="A378" s="1" t="s">
-        <v>17</v>
+        <v>382</v>
       </c>
       <c r="B378">
         <v>12042</v>
@@ -10178,12 +10472,12 @@
         <v>218162</v>
       </c>
       <c r="G378" t="s">
-        <v>17</v>
+        <v>382</v>
       </c>
     </row>
     <row r="379" spans="1:7">
       <c r="A379" s="1" t="s">
-        <v>18</v>
+        <v>383</v>
       </c>
       <c r="B379">
         <v>12058</v>
@@ -10201,12 +10495,12 @@
         <v>218162</v>
       </c>
       <c r="G379" t="s">
-        <v>18</v>
+        <v>383</v>
       </c>
     </row>
     <row r="380" spans="1:7">
       <c r="A380" s="1" t="s">
-        <v>19</v>
+        <v>384</v>
       </c>
       <c r="B380">
         <v>12097</v>
@@ -10224,12 +10518,12 @@
         <v>218162</v>
       </c>
       <c r="G380" t="s">
-        <v>19</v>
+        <v>384</v>
       </c>
     </row>
     <row r="381" spans="1:7">
       <c r="A381" s="1" t="s">
-        <v>20</v>
+        <v>385</v>
       </c>
       <c r="B381">
         <v>12132</v>
@@ -10247,12 +10541,12 @@
         <v>218162</v>
       </c>
       <c r="G381" t="s">
-        <v>20</v>
+        <v>385</v>
       </c>
     </row>
     <row r="382" spans="1:7">
       <c r="A382" s="1" t="s">
-        <v>21</v>
+        <v>386</v>
       </c>
       <c r="B382">
         <v>12283</v>
@@ -10270,12 +10564,12 @@
         <v>218162</v>
       </c>
       <c r="G382" t="s">
-        <v>21</v>
+        <v>386</v>
       </c>
     </row>
     <row r="383" spans="1:7">
       <c r="A383" s="1" t="s">
-        <v>22</v>
+        <v>387</v>
       </c>
       <c r="B383">
         <v>12392</v>
@@ -10293,12 +10587,12 @@
         <v>218162</v>
       </c>
       <c r="G383" t="s">
-        <v>22</v>
+        <v>387</v>
       </c>
     </row>
     <row r="384" spans="1:7">
       <c r="A384" s="1" t="s">
-        <v>23</v>
+        <v>388</v>
       </c>
       <c r="B384">
         <v>12469</v>
@@ -10316,12 +10610,12 @@
         <v>218162</v>
       </c>
       <c r="G384" t="s">
-        <v>23</v>
+        <v>388</v>
       </c>
     </row>
     <row r="385" spans="1:7">
       <c r="A385" s="1" t="s">
-        <v>24</v>
+        <v>389</v>
       </c>
       <c r="B385">
         <v>12535</v>
@@ -10339,12 +10633,12 @@
         <v>218162</v>
       </c>
       <c r="G385" t="s">
-        <v>24</v>
+        <v>389</v>
       </c>
     </row>
     <row r="386" spans="1:7">
       <c r="A386" s="1" t="s">
-        <v>25</v>
+        <v>390</v>
       </c>
       <c r="B386">
         <v>12603</v>
@@ -10362,12 +10656,12 @@
         <v>218162</v>
       </c>
       <c r="G386" t="s">
-        <v>25</v>
+        <v>390</v>
       </c>
     </row>
     <row r="387" spans="1:7">
       <c r="A387" s="1" t="s">
-        <v>26</v>
+        <v>391</v>
       </c>
       <c r="B387">
         <v>12621</v>
@@ -10385,12 +10679,12 @@
         <v>218162</v>
       </c>
       <c r="G387" t="s">
-        <v>26</v>
+        <v>391</v>
       </c>
     </row>
     <row r="388" spans="1:7">
       <c r="A388" s="1" t="s">
-        <v>27</v>
+        <v>392</v>
       </c>
       <c r="B388">
         <v>12672</v>
@@ -10408,12 +10702,12 @@
         <v>218162</v>
       </c>
       <c r="G388" t="s">
-        <v>27</v>
+        <v>392</v>
       </c>
     </row>
     <row r="389" spans="1:7">
       <c r="A389" s="1" t="s">
-        <v>28</v>
+        <v>393</v>
       </c>
       <c r="B389">
         <v>12781</v>
@@ -10431,12 +10725,12 @@
         <v>218162</v>
       </c>
       <c r="G389" t="s">
-        <v>28</v>
+        <v>393</v>
       </c>
     </row>
     <row r="390" spans="1:7">
       <c r="A390" s="1" t="s">
-        <v>29</v>
+        <v>394</v>
       </c>
       <c r="B390">
         <v>12851</v>
@@ -10454,12 +10748,12 @@
         <v>218162</v>
       </c>
       <c r="G390" t="s">
-        <v>29</v>
+        <v>394</v>
       </c>
     </row>
     <row r="391" spans="1:7">
       <c r="A391" s="1" t="s">
-        <v>30</v>
+        <v>395</v>
       </c>
       <c r="B391">
         <v>12979</v>
@@ -10477,12 +10771,12 @@
         <v>218162</v>
       </c>
       <c r="G391" t="s">
-        <v>30</v>
+        <v>395</v>
       </c>
     </row>
     <row r="392" spans="1:7">
       <c r="A392" s="1" t="s">
-        <v>31</v>
+        <v>396</v>
       </c>
       <c r="B392">
         <v>13062</v>
@@ -10500,12 +10794,12 @@
         <v>218162</v>
       </c>
       <c r="G392" t="s">
-        <v>31</v>
+        <v>396</v>
       </c>
     </row>
     <row r="393" spans="1:7">
       <c r="A393" s="1" t="s">
-        <v>32</v>
+        <v>397</v>
       </c>
       <c r="B393">
         <v>13101</v>
@@ -10523,12 +10817,12 @@
         <v>218162</v>
       </c>
       <c r="G393" t="s">
-        <v>32</v>
+        <v>397</v>
       </c>
     </row>
     <row r="394" spans="1:7">
       <c r="A394" s="1" t="s">
-        <v>33</v>
+        <v>398</v>
       </c>
       <c r="B394">
         <v>13128</v>
@@ -10546,12 +10840,12 @@
         <v>218162</v>
       </c>
       <c r="G394" t="s">
-        <v>33</v>
+        <v>398</v>
       </c>
     </row>
     <row r="395" spans="1:7">
       <c r="A395" s="1" t="s">
-        <v>34</v>
+        <v>399</v>
       </c>
       <c r="B395">
         <v>13169</v>
@@ -10569,12 +10863,12 @@
         <v>218162</v>
       </c>
       <c r="G395" t="s">
-        <v>34</v>
+        <v>399</v>
       </c>
     </row>
     <row r="396" spans="1:7">
       <c r="A396" s="1" t="s">
-        <v>35</v>
+        <v>400</v>
       </c>
       <c r="B396">
         <v>13245</v>
@@ -10592,12 +10886,12 @@
         <v>218162</v>
       </c>
       <c r="G396" t="s">
-        <v>35</v>
+        <v>400</v>
       </c>
     </row>
     <row r="397" spans="1:7">
       <c r="A397" s="1" t="s">
-        <v>36</v>
+        <v>401</v>
       </c>
       <c r="B397">
         <v>13285</v>
@@ -10615,12 +10909,12 @@
         <v>218162</v>
       </c>
       <c r="G397" t="s">
-        <v>36</v>
+        <v>401</v>
       </c>
     </row>
     <row r="398" spans="1:7">
       <c r="A398" s="1" t="s">
-        <v>37</v>
+        <v>402</v>
       </c>
       <c r="B398">
         <v>13320</v>
@@ -10638,12 +10932,12 @@
         <v>218162</v>
       </c>
       <c r="G398" t="s">
-        <v>37</v>
+        <v>402</v>
       </c>
     </row>
     <row r="399" spans="1:7">
       <c r="A399" s="1" t="s">
-        <v>38</v>
+        <v>403</v>
       </c>
       <c r="B399">
         <v>13413</v>
@@ -10661,12 +10955,12 @@
         <v>218162</v>
       </c>
       <c r="G399" t="s">
-        <v>38</v>
+        <v>403</v>
       </c>
     </row>
     <row r="400" spans="1:7">
       <c r="A400" s="1" t="s">
-        <v>39</v>
+        <v>404</v>
       </c>
       <c r="B400">
         <v>13486</v>
@@ -10684,12 +10978,12 @@
         <v>218162</v>
       </c>
       <c r="G400" t="s">
-        <v>39</v>
+        <v>404</v>
       </c>
     </row>
     <row r="401" spans="1:7">
       <c r="A401" s="1" t="s">
-        <v>40</v>
+        <v>405</v>
       </c>
       <c r="B401">
         <v>13513</v>
@@ -10707,12 +11001,12 @@
         <v>218162</v>
       </c>
       <c r="G401" t="s">
-        <v>40</v>
+        <v>405</v>
       </c>
     </row>
     <row r="402" spans="1:7">
       <c r="A402" s="1" t="s">
-        <v>41</v>
+        <v>406</v>
       </c>
       <c r="B402">
         <v>13545</v>
@@ -10730,12 +11024,12 @@
         <v>218162</v>
       </c>
       <c r="G402" t="s">
-        <v>41</v>
+        <v>406</v>
       </c>
     </row>
     <row r="403" spans="1:7">
       <c r="A403" s="1" t="s">
-        <v>42</v>
+        <v>407</v>
       </c>
       <c r="B403">
         <v>13621</v>
@@ -10753,12 +11047,12 @@
         <v>218162</v>
       </c>
       <c r="G403" t="s">
-        <v>42</v>
+        <v>407</v>
       </c>
     </row>
     <row r="404" spans="1:7">
       <c r="A404" s="1" t="s">
-        <v>43</v>
+        <v>408</v>
       </c>
       <c r="B404">
         <v>13701</v>
@@ -10776,12 +11070,12 @@
         <v>218162</v>
       </c>
       <c r="G404" t="s">
-        <v>43</v>
+        <v>408</v>
       </c>
     </row>
     <row r="405" spans="1:7">
       <c r="A405" s="1" t="s">
-        <v>44</v>
+        <v>409</v>
       </c>
       <c r="B405">
         <v>13754</v>
@@ -10799,12 +11093,12 @@
         <v>218162</v>
       </c>
       <c r="G405" t="s">
-        <v>44</v>
+        <v>409</v>
       </c>
     </row>
     <row r="406" spans="1:7">
       <c r="A406" s="1" t="s">
-        <v>45</v>
+        <v>410</v>
       </c>
       <c r="B406">
         <v>13809</v>
@@ -10822,12 +11116,12 @@
         <v>218162</v>
       </c>
       <c r="G406" t="s">
-        <v>45</v>
+        <v>410</v>
       </c>
     </row>
     <row r="407" spans="1:7">
       <c r="A407" s="1" t="s">
-        <v>46</v>
+        <v>411</v>
       </c>
       <c r="B407">
         <v>13850</v>
@@ -10845,12 +11139,12 @@
         <v>218162</v>
       </c>
       <c r="G407" t="s">
-        <v>46</v>
+        <v>411</v>
       </c>
     </row>
     <row r="408" spans="1:7">
       <c r="A408" s="1" t="s">
-        <v>47</v>
+        <v>412</v>
       </c>
       <c r="B408">
         <v>13868</v>
@@ -10868,12 +11162,12 @@
         <v>218162</v>
       </c>
       <c r="G408" t="s">
-        <v>47</v>
+        <v>412</v>
       </c>
     </row>
     <row r="409" spans="1:7">
       <c r="A409" s="1" t="s">
-        <v>48</v>
+        <v>413</v>
       </c>
       <c r="B409">
         <v>13918</v>
@@ -10891,12 +11185,12 @@
         <v>218162</v>
       </c>
       <c r="G409" t="s">
-        <v>48</v>
+        <v>413</v>
       </c>
     </row>
     <row r="410" spans="1:7">
       <c r="A410" s="1" t="s">
-        <v>49</v>
+        <v>414</v>
       </c>
       <c r="B410">
         <v>13977</v>
@@ -10914,12 +11208,12 @@
         <v>218162</v>
       </c>
       <c r="G410" t="s">
-        <v>49</v>
+        <v>414</v>
       </c>
     </row>
     <row r="411" spans="1:7">
       <c r="A411" s="1" t="s">
-        <v>50</v>
+        <v>415</v>
       </c>
       <c r="B411">
         <v>14008</v>
@@ -10937,12 +11231,12 @@
         <v>218162</v>
       </c>
       <c r="G411" t="s">
-        <v>50</v>
+        <v>415</v>
       </c>
     </row>
     <row r="412" spans="1:7">
       <c r="A412" s="1" t="s">
-        <v>51</v>
+        <v>416</v>
       </c>
       <c r="B412">
         <v>14068</v>
@@ -10960,12 +11254,12 @@
         <v>218162</v>
       </c>
       <c r="G412" t="s">
-        <v>51</v>
+        <v>416</v>
       </c>
     </row>
     <row r="413" spans="1:7">
       <c r="A413" s="1" t="s">
-        <v>52</v>
+        <v>417</v>
       </c>
       <c r="B413">
         <v>14114</v>
@@ -10983,12 +11277,12 @@
         <v>218162</v>
       </c>
       <c r="G413" t="s">
-        <v>52</v>
+        <v>417</v>
       </c>
     </row>
     <row r="414" spans="1:7">
       <c r="A414" s="1" t="s">
-        <v>53</v>
+        <v>418</v>
       </c>
       <c r="B414">
         <v>14159</v>
@@ -11006,12 +11300,12 @@
         <v>218162</v>
       </c>
       <c r="G414" t="s">
-        <v>53</v>
+        <v>418</v>
       </c>
     </row>
     <row r="415" spans="1:7">
       <c r="A415" s="1" t="s">
-        <v>54</v>
+        <v>419</v>
       </c>
       <c r="B415">
         <v>14172</v>
@@ -11029,12 +11323,12 @@
         <v>218162</v>
       </c>
       <c r="G415" t="s">
-        <v>54</v>
+        <v>419</v>
       </c>
     </row>
     <row r="416" spans="1:7">
       <c r="A416" s="1" t="s">
-        <v>55</v>
+        <v>420</v>
       </c>
       <c r="B416">
         <v>14202</v>
@@ -11052,12 +11346,12 @@
         <v>218162</v>
       </c>
       <c r="G416" t="s">
-        <v>55</v>
+        <v>420</v>
       </c>
     </row>
     <row r="417" spans="1:7">
       <c r="A417" s="1" t="s">
-        <v>56</v>
+        <v>421</v>
       </c>
       <c r="B417">
         <v>14202</v>
@@ -11075,12 +11369,12 @@
         <v>218162</v>
       </c>
       <c r="G417" t="s">
-        <v>56</v>
+        <v>421</v>
       </c>
     </row>
     <row r="418" spans="1:7">
       <c r="A418" s="1" t="s">
-        <v>57</v>
+        <v>422</v>
       </c>
       <c r="B418">
         <v>14329</v>
@@ -11098,12 +11392,12 @@
         <v>218162</v>
       </c>
       <c r="G418" t="s">
-        <v>57</v>
+        <v>422</v>
       </c>
     </row>
     <row r="419" spans="1:7">
       <c r="A419" s="1" t="s">
-        <v>58</v>
+        <v>423</v>
       </c>
       <c r="B419">
         <v>14366</v>
@@ -11121,12 +11415,12 @@
         <v>218162</v>
       </c>
       <c r="G419" t="s">
-        <v>58</v>
+        <v>423</v>
       </c>
     </row>
     <row r="420" spans="1:7">
       <c r="A420" s="1" t="s">
-        <v>59</v>
+        <v>424</v>
       </c>
       <c r="B420">
         <v>14420</v>
@@ -11144,12 +11438,12 @@
         <v>218162</v>
       </c>
       <c r="G420" t="s">
-        <v>59</v>
+        <v>424</v>
       </c>
     </row>
     <row r="421" spans="1:7">
       <c r="A421" s="1" t="s">
-        <v>60</v>
+        <v>425</v>
       </c>
       <c r="B421">
         <v>14486</v>
@@ -11167,12 +11461,12 @@
         <v>218162</v>
       </c>
       <c r="G421" t="s">
-        <v>60</v>
+        <v>425</v>
       </c>
     </row>
     <row r="422" spans="1:7">
       <c r="A422" s="1" t="s">
-        <v>61</v>
+        <v>426</v>
       </c>
       <c r="B422">
         <v>14492</v>
@@ -11190,12 +11484,12 @@
         <v>218162</v>
       </c>
       <c r="G422" t="s">
-        <v>61</v>
+        <v>426</v>
       </c>
     </row>
     <row r="423" spans="1:7">
       <c r="A423" s="1" t="s">
-        <v>62</v>
+        <v>427</v>
       </c>
       <c r="B423">
         <v>14501</v>
@@ -11213,12 +11507,12 @@
         <v>218162</v>
       </c>
       <c r="G423" t="s">
-        <v>62</v>
+        <v>427</v>
       </c>
     </row>
     <row r="424" spans="1:7">
       <c r="A424" s="1" t="s">
-        <v>63</v>
+        <v>428</v>
       </c>
       <c r="B424">
         <v>14544</v>
@@ -11236,12 +11530,12 @@
         <v>218162</v>
       </c>
       <c r="G424" t="s">
-        <v>63</v>
+        <v>428</v>
       </c>
     </row>
     <row r="425" spans="1:7">
       <c r="A425" s="1" t="s">
-        <v>64</v>
+        <v>429</v>
       </c>
       <c r="B425">
         <v>14575</v>
@@ -11259,12 +11553,12 @@
         <v>218162</v>
       </c>
       <c r="G425" t="s">
-        <v>64</v>
+        <v>429</v>
       </c>
     </row>
     <row r="426" spans="1:7">
       <c r="A426" s="1" t="s">
-        <v>65</v>
+        <v>430</v>
       </c>
       <c r="B426">
         <v>14626</v>
@@ -11282,12 +11576,12 @@
         <v>218162</v>
       </c>
       <c r="G426" t="s">
-        <v>65</v>
+        <v>430</v>
       </c>
     </row>
     <row r="427" spans="1:7">
       <c r="A427" s="1" t="s">
-        <v>66</v>
+        <v>431</v>
       </c>
       <c r="B427">
         <v>14670</v>
@@ -11305,12 +11599,12 @@
         <v>218162</v>
       </c>
       <c r="G427" t="s">
-        <v>66</v>
+        <v>431</v>
       </c>
     </row>
     <row r="428" spans="1:7">
       <c r="A428" s="1" t="s">
-        <v>67</v>
+        <v>432</v>
       </c>
       <c r="B428">
         <v>14698</v>
@@ -11328,12 +11622,12 @@
         <v>218162</v>
       </c>
       <c r="G428" t="s">
-        <v>67</v>
+        <v>432</v>
       </c>
     </row>
     <row r="429" spans="1:7">
       <c r="A429" s="1" t="s">
-        <v>68</v>
+        <v>433</v>
       </c>
       <c r="B429">
         <v>14715</v>
@@ -11351,12 +11645,12 @@
         <v>218162</v>
       </c>
       <c r="G429" t="s">
-        <v>68</v>
+        <v>433</v>
       </c>
     </row>
     <row r="430" spans="1:7">
       <c r="A430" s="1" t="s">
-        <v>69</v>
+        <v>434</v>
       </c>
       <c r="B430">
         <v>14740</v>
@@ -11374,12 +11668,12 @@
         <v>218162</v>
       </c>
       <c r="G430" t="s">
-        <v>69</v>
+        <v>434</v>
       </c>
     </row>
     <row r="431" spans="1:7">
       <c r="A431" s="1" t="s">
-        <v>70</v>
+        <v>435</v>
       </c>
       <c r="B431">
         <v>14794</v>
@@ -11397,12 +11691,12 @@
         <v>218162</v>
       </c>
       <c r="G431" t="s">
-        <v>70</v>
+        <v>435</v>
       </c>
     </row>
     <row r="432" spans="1:7">
       <c r="A432" s="1" t="s">
-        <v>71</v>
+        <v>436</v>
       </c>
       <c r="B432">
         <v>14845</v>
@@ -11420,12 +11714,12 @@
         <v>218162</v>
       </c>
       <c r="G432" t="s">
-        <v>71</v>
+        <v>436</v>
       </c>
     </row>
     <row r="433" spans="1:7">
       <c r="A433" s="1" t="s">
-        <v>72</v>
+        <v>437</v>
       </c>
       <c r="B433">
         <v>14908</v>
@@ -11443,12 +11737,12 @@
         <v>218162</v>
       </c>
       <c r="G433" t="s">
-        <v>72</v>
+        <v>437</v>
       </c>
     </row>
     <row r="434" spans="1:7">
       <c r="A434" s="1" t="s">
-        <v>73</v>
+        <v>438</v>
       </c>
       <c r="B434">
         <v>14908</v>
@@ -11466,12 +11760,12 @@
         <v>218162</v>
       </c>
       <c r="G434" t="s">
-        <v>73</v>
+        <v>438</v>
       </c>
     </row>
     <row r="435" spans="1:7">
       <c r="A435" s="1" t="s">
-        <v>74</v>
+        <v>439</v>
       </c>
       <c r="B435">
         <v>14908</v>
@@ -11489,12 +11783,12 @@
         <v>218162</v>
       </c>
       <c r="G435" t="s">
-        <v>74</v>
+        <v>439</v>
       </c>
     </row>
     <row r="436" spans="1:7">
       <c r="A436" s="1" t="s">
-        <v>75</v>
+        <v>440</v>
       </c>
       <c r="B436">
         <v>15002</v>
@@ -11512,12 +11806,12 @@
         <v>218162</v>
       </c>
       <c r="G436" t="s">
-        <v>75</v>
+        <v>440</v>
       </c>
     </row>
     <row r="437" spans="1:7">
       <c r="A437" s="1" t="s">
-        <v>76</v>
+        <v>441</v>
       </c>
       <c r="B437">
         <v>15048</v>
@@ -11535,12 +11829,12 @@
         <v>218162</v>
       </c>
       <c r="G437" t="s">
-        <v>76</v>
+        <v>441</v>
       </c>
     </row>
     <row r="438" spans="1:7">
       <c r="A438" s="1" t="s">
-        <v>77</v>
+        <v>442</v>
       </c>
       <c r="B438">
         <v>15077</v>
@@ -11558,12 +11852,12 @@
         <v>218162</v>
       </c>
       <c r="G438" t="s">
-        <v>77</v>
+        <v>442</v>
       </c>
     </row>
     <row r="439" spans="1:7">
       <c r="A439" s="1" t="s">
-        <v>78</v>
+        <v>443</v>
       </c>
       <c r="B439">
         <v>15115</v>
@@ -11581,12 +11875,12 @@
         <v>218162</v>
       </c>
       <c r="G439" t="s">
-        <v>78</v>
+        <v>443</v>
       </c>
     </row>
     <row r="440" spans="1:7">
       <c r="A440" s="1" t="s">
-        <v>79</v>
+        <v>444</v>
       </c>
       <c r="B440">
         <v>15146</v>
@@ -11604,12 +11898,12 @@
         <v>218162</v>
       </c>
       <c r="G440" t="s">
-        <v>79</v>
+        <v>444</v>
       </c>
     </row>
     <row r="441" spans="1:7">
       <c r="A441" s="1" t="s">
-        <v>80</v>
+        <v>445</v>
       </c>
       <c r="B441">
         <v>15157</v>
@@ -11627,12 +11921,12 @@
         <v>218162</v>
       </c>
       <c r="G441" t="s">
-        <v>80</v>
+        <v>445</v>
       </c>
     </row>
     <row r="442" spans="1:7">
       <c r="A442" s="1" t="s">
-        <v>81</v>
+        <v>446</v>
       </c>
       <c r="B442">
         <v>15195</v>
@@ -11650,12 +11944,12 @@
         <v>218162</v>
       </c>
       <c r="G442" t="s">
-        <v>81</v>
+        <v>446</v>
       </c>
     </row>
     <row r="443" spans="1:7">
       <c r="A443" s="1" t="s">
-        <v>82</v>
+        <v>447</v>
       </c>
       <c r="B443">
         <v>15221</v>
@@ -11673,12 +11967,12 @@
         <v>218162</v>
       </c>
       <c r="G443" t="s">
-        <v>82</v>
+        <v>447</v>
       </c>
     </row>
     <row r="444" spans="1:7">
       <c r="A444" s="1" t="s">
-        <v>83</v>
+        <v>448</v>
       </c>
       <c r="B444">
         <v>15235</v>
@@ -11696,12 +11990,12 @@
         <v>218162</v>
       </c>
       <c r="G444" t="s">
-        <v>83</v>
+        <v>448</v>
       </c>
     </row>
     <row r="445" spans="1:7">
       <c r="A445" s="1" t="s">
-        <v>84</v>
+        <v>449</v>
       </c>
       <c r="B445">
         <v>15263</v>
@@ -11719,12 +12013,12 @@
         <v>218162</v>
       </c>
       <c r="G445" t="s">
-        <v>84</v>
+        <v>449</v>
       </c>
     </row>
     <row r="446" spans="1:7">
       <c r="A446" s="1" t="s">
-        <v>85</v>
+        <v>450</v>
       </c>
       <c r="B446">
         <v>15374</v>
@@ -11742,12 +12036,12 @@
         <v>218162</v>
       </c>
       <c r="G446" t="s">
-        <v>85</v>
+        <v>450</v>
       </c>
     </row>
     <row r="447" spans="1:7">
       <c r="A447" s="1" t="s">
-        <v>86</v>
+        <v>451</v>
       </c>
       <c r="B447">
         <v>15418</v>
@@ -11765,12 +12059,12 @@
         <v>218162</v>
       </c>
       <c r="G447" t="s">
-        <v>86</v>
+        <v>451</v>
       </c>
     </row>
     <row r="448" spans="1:7">
       <c r="A448" s="1" t="s">
-        <v>87</v>
+        <v>452</v>
       </c>
       <c r="B448">
         <v>15497</v>
@@ -11788,12 +12082,12 @@
         <v>218162</v>
       </c>
       <c r="G448" t="s">
-        <v>87</v>
+        <v>452</v>
       </c>
     </row>
     <row r="449" spans="1:7">
       <c r="A449" s="1" t="s">
-        <v>88</v>
+        <v>453</v>
       </c>
       <c r="B449">
         <v>15572</v>
@@ -11811,12 +12105,12 @@
         <v>218162</v>
       </c>
       <c r="G449" t="s">
-        <v>88</v>
+        <v>453</v>
       </c>
     </row>
     <row r="450" spans="1:7">
       <c r="A450" s="1" t="s">
-        <v>89</v>
+        <v>454</v>
       </c>
       <c r="B450">
         <v>15597</v>
@@ -11834,12 +12128,12 @@
         <v>218162</v>
       </c>
       <c r="G450" t="s">
-        <v>89</v>
+        <v>454</v>
       </c>
     </row>
     <row r="451" spans="1:7">
       <c r="A451" s="1" t="s">
-        <v>90</v>
+        <v>455</v>
       </c>
       <c r="B451">
         <v>15618</v>
@@ -11857,12 +12151,12 @@
         <v>218162</v>
       </c>
       <c r="G451" t="s">
-        <v>90</v>
+        <v>455</v>
       </c>
     </row>
     <row r="452" spans="1:7">
       <c r="A452" s="1" t="s">
-        <v>91</v>
+        <v>456</v>
       </c>
       <c r="B452">
         <v>15618</v>
@@ -11880,7 +12174,283 @@
         <v>218162</v>
       </c>
       <c r="G452" t="s">
-        <v>91</v>
+        <v>456</v>
+      </c>
+    </row>
+    <row r="453" spans="1:7">
+      <c r="A453" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B453">
+        <v>15732</v>
+      </c>
+      <c r="C453">
+        <v>338</v>
+      </c>
+      <c r="D453">
+        <v>7</v>
+      </c>
+      <c r="E453">
+        <v>114</v>
+      </c>
+      <c r="F453">
+        <v>218162</v>
+      </c>
+      <c r="G453" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="454" spans="1:7">
+      <c r="A454" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B454">
+        <v>15793</v>
+      </c>
+      <c r="C454">
+        <v>339</v>
+      </c>
+      <c r="D454">
+        <v>1</v>
+      </c>
+      <c r="E454">
+        <v>61</v>
+      </c>
+      <c r="F454">
+        <v>218162</v>
+      </c>
+      <c r="G454" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="455" spans="1:7">
+      <c r="A455" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B455">
+        <v>15793</v>
+      </c>
+      <c r="C455">
+        <v>339</v>
+      </c>
+      <c r="D455">
+        <v>0</v>
+      </c>
+      <c r="E455">
+        <v>0</v>
+      </c>
+      <c r="F455">
+        <v>218162</v>
+      </c>
+      <c r="G455" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="456" spans="1:7">
+      <c r="A456" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B456">
+        <v>15894</v>
+      </c>
+      <c r="C456">
+        <v>341</v>
+      </c>
+      <c r="D456">
+        <v>2</v>
+      </c>
+      <c r="E456">
+        <v>101</v>
+      </c>
+      <c r="F456">
+        <v>218162</v>
+      </c>
+      <c r="G456" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="457" spans="1:7">
+      <c r="A457" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B457">
+        <v>15916</v>
+      </c>
+      <c r="C457">
+        <v>342</v>
+      </c>
+      <c r="D457">
+        <v>1</v>
+      </c>
+      <c r="E457">
+        <v>22</v>
+      </c>
+      <c r="F457">
+        <v>218162</v>
+      </c>
+      <c r="G457" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="458" spans="1:7">
+      <c r="A458" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B458">
+        <v>15951</v>
+      </c>
+      <c r="C458">
+        <v>342</v>
+      </c>
+      <c r="D458">
+        <v>0</v>
+      </c>
+      <c r="E458">
+        <v>35</v>
+      </c>
+      <c r="F458">
+        <v>218162</v>
+      </c>
+      <c r="G458" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="459" spans="1:7">
+      <c r="A459" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B459">
+        <v>16001</v>
+      </c>
+      <c r="C459">
+        <v>343</v>
+      </c>
+      <c r="D459">
+        <v>1</v>
+      </c>
+      <c r="E459">
+        <v>50</v>
+      </c>
+      <c r="F459">
+        <v>218162</v>
+      </c>
+      <c r="G459" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="460" spans="1:7">
+      <c r="A460" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B460">
+        <v>16057</v>
+      </c>
+      <c r="C460">
+        <v>345</v>
+      </c>
+      <c r="D460">
+        <v>2</v>
+      </c>
+      <c r="E460">
+        <v>56</v>
+      </c>
+      <c r="F460">
+        <v>218162</v>
+      </c>
+      <c r="G460" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="461" spans="1:7">
+      <c r="A461" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B461">
+        <v>16094</v>
+      </c>
+      <c r="C461">
+        <v>354</v>
+      </c>
+      <c r="D461">
+        <v>9</v>
+      </c>
+      <c r="E461">
+        <v>37</v>
+      </c>
+      <c r="F461">
+        <v>218162</v>
+      </c>
+      <c r="G461" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="462" spans="1:7">
+      <c r="A462" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B462">
+        <v>16116</v>
+      </c>
+      <c r="C462">
+        <v>355</v>
+      </c>
+      <c r="D462">
+        <v>1</v>
+      </c>
+      <c r="E462">
+        <v>22</v>
+      </c>
+      <c r="F462">
+        <v>218162</v>
+      </c>
+      <c r="G462" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="463" spans="1:7">
+      <c r="A463" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B463">
+        <v>16151</v>
+      </c>
+      <c r="C463">
+        <v>356</v>
+      </c>
+      <c r="D463">
+        <v>1</v>
+      </c>
+      <c r="E463">
+        <v>35</v>
+      </c>
+      <c r="F463">
+        <v>218162</v>
+      </c>
+      <c r="G463" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="464" spans="1:7">
+      <c r="A464" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B464">
+        <v>16151</v>
+      </c>
+      <c r="C464">
+        <v>356</v>
+      </c>
+      <c r="D464">
+        <v>0</v>
+      </c>
+      <c r="E464">
+        <v>0</v>
+      </c>
+      <c r="F464">
+        <v>218162</v>
+      </c>
+      <c r="G464" t="s">
+        <v>468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
config the main error
</commit_message>
<xml_diff>
--- a/data/dados_Juazeiro_BA.xlsx
+++ b/data/dados_Juazeiro_BA.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F501"/>
+  <dimension ref="A1:F580"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11460,6 +11460,1744 @@
         <v>218162</v>
       </c>
     </row>
+    <row r="502">
+      <c r="A502" s="1" t="inlineStr">
+        <is>
+          <t>05/ago/2021</t>
+        </is>
+      </c>
+      <c r="B502" t="n">
+        <v>16927</v>
+      </c>
+      <c r="C502" t="n">
+        <v>389</v>
+      </c>
+      <c r="D502" t="n">
+        <v>0</v>
+      </c>
+      <c r="E502" t="n">
+        <v>0</v>
+      </c>
+      <c r="F502" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" s="1" t="inlineStr">
+        <is>
+          <t>06/ago/2021</t>
+        </is>
+      </c>
+      <c r="B503" t="n">
+        <v>16927</v>
+      </c>
+      <c r="C503" t="n">
+        <v>389</v>
+      </c>
+      <c r="D503" t="n">
+        <v>0</v>
+      </c>
+      <c r="E503" t="n">
+        <v>0</v>
+      </c>
+      <c r="F503" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" s="1" t="inlineStr">
+        <is>
+          <t>07/ago/2021</t>
+        </is>
+      </c>
+      <c r="B504" t="n">
+        <v>16927</v>
+      </c>
+      <c r="C504" t="n">
+        <v>389</v>
+      </c>
+      <c r="D504" t="n">
+        <v>0</v>
+      </c>
+      <c r="E504" t="n">
+        <v>0</v>
+      </c>
+      <c r="F504" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" s="1" t="inlineStr">
+        <is>
+          <t>08/ago/2021</t>
+        </is>
+      </c>
+      <c r="B505" t="n">
+        <v>16927</v>
+      </c>
+      <c r="C505" t="n">
+        <v>389</v>
+      </c>
+      <c r="D505" t="n">
+        <v>0</v>
+      </c>
+      <c r="E505" t="n">
+        <v>0</v>
+      </c>
+      <c r="F505" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" s="1" t="inlineStr">
+        <is>
+          <t>09/ago/2021</t>
+        </is>
+      </c>
+      <c r="B506" t="n">
+        <v>16927</v>
+      </c>
+      <c r="C506" t="n">
+        <v>389</v>
+      </c>
+      <c r="D506" t="n">
+        <v>0</v>
+      </c>
+      <c r="E506" t="n">
+        <v>0</v>
+      </c>
+      <c r="F506" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" s="1" t="inlineStr">
+        <is>
+          <t>10/ago/2021</t>
+        </is>
+      </c>
+      <c r="B507" t="n">
+        <v>16927</v>
+      </c>
+      <c r="C507" t="n">
+        <v>389</v>
+      </c>
+      <c r="D507" t="n">
+        <v>0</v>
+      </c>
+      <c r="E507" t="n">
+        <v>0</v>
+      </c>
+      <c r="F507" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" s="1" t="inlineStr">
+        <is>
+          <t>11/ago/2021</t>
+        </is>
+      </c>
+      <c r="B508" t="n">
+        <v>16927</v>
+      </c>
+      <c r="C508" t="n">
+        <v>389</v>
+      </c>
+      <c r="D508" t="n">
+        <v>0</v>
+      </c>
+      <c r="E508" t="n">
+        <v>0</v>
+      </c>
+      <c r="F508" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" s="1" t="inlineStr">
+        <is>
+          <t>12/ago/2021</t>
+        </is>
+      </c>
+      <c r="B509" t="n">
+        <v>16927</v>
+      </c>
+      <c r="C509" t="n">
+        <v>389</v>
+      </c>
+      <c r="D509" t="n">
+        <v>0</v>
+      </c>
+      <c r="E509" t="n">
+        <v>0</v>
+      </c>
+      <c r="F509" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" s="1" t="inlineStr">
+        <is>
+          <t>13/ago/2021</t>
+        </is>
+      </c>
+      <c r="B510" t="n">
+        <v>17142</v>
+      </c>
+      <c r="C510" t="n">
+        <v>389</v>
+      </c>
+      <c r="D510" t="n">
+        <v>0</v>
+      </c>
+      <c r="E510" t="n">
+        <v>215</v>
+      </c>
+      <c r="F510" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" s="1" t="inlineStr">
+        <is>
+          <t>14/ago/2021</t>
+        </is>
+      </c>
+      <c r="B511" t="n">
+        <v>17142</v>
+      </c>
+      <c r="C511" t="n">
+        <v>389</v>
+      </c>
+      <c r="D511" t="n">
+        <v>0</v>
+      </c>
+      <c r="E511" t="n">
+        <v>0</v>
+      </c>
+      <c r="F511" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" s="1" t="inlineStr">
+        <is>
+          <t>15/ago/2021</t>
+        </is>
+      </c>
+      <c r="B512" t="n">
+        <v>17166</v>
+      </c>
+      <c r="C512" t="n">
+        <v>389</v>
+      </c>
+      <c r="D512" t="n">
+        <v>0</v>
+      </c>
+      <c r="E512" t="n">
+        <v>24</v>
+      </c>
+      <c r="F512" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" s="1" t="inlineStr">
+        <is>
+          <t>16/ago/2021</t>
+        </is>
+      </c>
+      <c r="B513" t="n">
+        <v>17166</v>
+      </c>
+      <c r="C513" t="n">
+        <v>389</v>
+      </c>
+      <c r="D513" t="n">
+        <v>0</v>
+      </c>
+      <c r="E513" t="n">
+        <v>0</v>
+      </c>
+      <c r="F513" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" s="1" t="inlineStr">
+        <is>
+          <t>17/ago/2021</t>
+        </is>
+      </c>
+      <c r="B514" t="n">
+        <v>17171</v>
+      </c>
+      <c r="C514" t="n">
+        <v>390</v>
+      </c>
+      <c r="D514" t="n">
+        <v>1</v>
+      </c>
+      <c r="E514" t="n">
+        <v>5</v>
+      </c>
+      <c r="F514" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" s="1" t="inlineStr">
+        <is>
+          <t>18/ago/2021</t>
+        </is>
+      </c>
+      <c r="B515" t="n">
+        <v>17176</v>
+      </c>
+      <c r="C515" t="n">
+        <v>390</v>
+      </c>
+      <c r="D515" t="n">
+        <v>0</v>
+      </c>
+      <c r="E515" t="n">
+        <v>5</v>
+      </c>
+      <c r="F515" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" s="1" t="inlineStr">
+        <is>
+          <t>19/ago/2021</t>
+        </is>
+      </c>
+      <c r="B516" t="n">
+        <v>17176</v>
+      </c>
+      <c r="C516" t="n">
+        <v>390</v>
+      </c>
+      <c r="D516" t="n">
+        <v>0</v>
+      </c>
+      <c r="E516" t="n">
+        <v>0</v>
+      </c>
+      <c r="F516" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" s="1" t="inlineStr">
+        <is>
+          <t>20/ago/2021</t>
+        </is>
+      </c>
+      <c r="B517" t="n">
+        <v>17176</v>
+      </c>
+      <c r="C517" t="n">
+        <v>390</v>
+      </c>
+      <c r="D517" t="n">
+        <v>0</v>
+      </c>
+      <c r="E517" t="n">
+        <v>0</v>
+      </c>
+      <c r="F517" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" s="1" t="inlineStr">
+        <is>
+          <t>21/ago/2021</t>
+        </is>
+      </c>
+      <c r="B518" t="n">
+        <v>17202</v>
+      </c>
+      <c r="C518" t="n">
+        <v>390</v>
+      </c>
+      <c r="D518" t="n">
+        <v>0</v>
+      </c>
+      <c r="E518" t="n">
+        <v>26</v>
+      </c>
+      <c r="F518" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" s="1" t="inlineStr">
+        <is>
+          <t>22/ago/2021</t>
+        </is>
+      </c>
+      <c r="B519" t="n">
+        <v>17213</v>
+      </c>
+      <c r="C519" t="n">
+        <v>390</v>
+      </c>
+      <c r="D519" t="n">
+        <v>0</v>
+      </c>
+      <c r="E519" t="n">
+        <v>11</v>
+      </c>
+      <c r="F519" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" s="1" t="inlineStr">
+        <is>
+          <t>23/ago/2021</t>
+        </is>
+      </c>
+      <c r="B520" t="n">
+        <v>17213</v>
+      </c>
+      <c r="C520" t="n">
+        <v>390</v>
+      </c>
+      <c r="D520" t="n">
+        <v>0</v>
+      </c>
+      <c r="E520" t="n">
+        <v>0</v>
+      </c>
+      <c r="F520" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" s="1" t="inlineStr">
+        <is>
+          <t>24/ago/2021</t>
+        </is>
+      </c>
+      <c r="B521" t="n">
+        <v>17234</v>
+      </c>
+      <c r="C521" t="n">
+        <v>391</v>
+      </c>
+      <c r="D521" t="n">
+        <v>1</v>
+      </c>
+      <c r="E521" t="n">
+        <v>21</v>
+      </c>
+      <c r="F521" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" s="1" t="inlineStr">
+        <is>
+          <t>25/ago/2021</t>
+        </is>
+      </c>
+      <c r="B522" t="n">
+        <v>17234</v>
+      </c>
+      <c r="C522" t="n">
+        <v>391</v>
+      </c>
+      <c r="D522" t="n">
+        <v>0</v>
+      </c>
+      <c r="E522" t="n">
+        <v>0</v>
+      </c>
+      <c r="F522" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" s="1" t="inlineStr">
+        <is>
+          <t>26/ago/2021</t>
+        </is>
+      </c>
+      <c r="B523" t="n">
+        <v>17271</v>
+      </c>
+      <c r="C523" t="n">
+        <v>391</v>
+      </c>
+      <c r="D523" t="n">
+        <v>0</v>
+      </c>
+      <c r="E523" t="n">
+        <v>37</v>
+      </c>
+      <c r="F523" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" s="1" t="inlineStr">
+        <is>
+          <t>27/ago/2021</t>
+        </is>
+      </c>
+      <c r="B524" t="n">
+        <v>17271</v>
+      </c>
+      <c r="C524" t="n">
+        <v>391</v>
+      </c>
+      <c r="D524" t="n">
+        <v>0</v>
+      </c>
+      <c r="E524" t="n">
+        <v>0</v>
+      </c>
+      <c r="F524" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" s="1" t="inlineStr">
+        <is>
+          <t>28/ago/2021</t>
+        </is>
+      </c>
+      <c r="B525" t="n">
+        <v>17287</v>
+      </c>
+      <c r="C525" t="n">
+        <v>391</v>
+      </c>
+      <c r="D525" t="n">
+        <v>0</v>
+      </c>
+      <c r="E525" t="n">
+        <v>16</v>
+      </c>
+      <c r="F525" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" s="1" t="inlineStr">
+        <is>
+          <t>29/ago/2021</t>
+        </is>
+      </c>
+      <c r="B526" t="n">
+        <v>17287</v>
+      </c>
+      <c r="C526" t="n">
+        <v>391</v>
+      </c>
+      <c r="D526" t="n">
+        <v>0</v>
+      </c>
+      <c r="E526" t="n">
+        <v>0</v>
+      </c>
+      <c r="F526" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" s="1" t="inlineStr">
+        <is>
+          <t>30/ago/2021</t>
+        </is>
+      </c>
+      <c r="B527" t="n">
+        <v>17287</v>
+      </c>
+      <c r="C527" t="n">
+        <v>391</v>
+      </c>
+      <c r="D527" t="n">
+        <v>0</v>
+      </c>
+      <c r="E527" t="n">
+        <v>0</v>
+      </c>
+      <c r="F527" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" s="1" t="inlineStr">
+        <is>
+          <t>31/ago/2021</t>
+        </is>
+      </c>
+      <c r="B528" t="n">
+        <v>17287</v>
+      </c>
+      <c r="C528" t="n">
+        <v>391</v>
+      </c>
+      <c r="D528" t="n">
+        <v>0</v>
+      </c>
+      <c r="E528" t="n">
+        <v>0</v>
+      </c>
+      <c r="F528" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" s="1" t="inlineStr">
+        <is>
+          <t>01/set/2021</t>
+        </is>
+      </c>
+      <c r="B529" t="n">
+        <v>17312</v>
+      </c>
+      <c r="C529" t="n">
+        <v>391</v>
+      </c>
+      <c r="D529" t="n">
+        <v>0</v>
+      </c>
+      <c r="E529" t="n">
+        <v>25</v>
+      </c>
+      <c r="F529" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" s="1" t="inlineStr">
+        <is>
+          <t>02/set/2021</t>
+        </is>
+      </c>
+      <c r="B530" t="n">
+        <v>17326</v>
+      </c>
+      <c r="C530" t="n">
+        <v>391</v>
+      </c>
+      <c r="D530" t="n">
+        <v>0</v>
+      </c>
+      <c r="E530" t="n">
+        <v>14</v>
+      </c>
+      <c r="F530" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" s="1" t="inlineStr">
+        <is>
+          <t>03/set/2021</t>
+        </is>
+      </c>
+      <c r="B531" t="n">
+        <v>17326</v>
+      </c>
+      <c r="C531" t="n">
+        <v>391</v>
+      </c>
+      <c r="D531" t="n">
+        <v>0</v>
+      </c>
+      <c r="E531" t="n">
+        <v>0</v>
+      </c>
+      <c r="F531" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" s="1" t="inlineStr">
+        <is>
+          <t>04/set/2021</t>
+        </is>
+      </c>
+      <c r="B532" t="n">
+        <v>17326</v>
+      </c>
+      <c r="C532" t="n">
+        <v>391</v>
+      </c>
+      <c r="D532" t="n">
+        <v>0</v>
+      </c>
+      <c r="E532" t="n">
+        <v>0</v>
+      </c>
+      <c r="F532" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" s="1" t="inlineStr">
+        <is>
+          <t>05/set/2021</t>
+        </is>
+      </c>
+      <c r="B533" t="n">
+        <v>17326</v>
+      </c>
+      <c r="C533" t="n">
+        <v>391</v>
+      </c>
+      <c r="D533" t="n">
+        <v>0</v>
+      </c>
+      <c r="E533" t="n">
+        <v>0</v>
+      </c>
+      <c r="F533" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" s="1" t="inlineStr">
+        <is>
+          <t>06/set/2021</t>
+        </is>
+      </c>
+      <c r="B534" t="n">
+        <v>17326</v>
+      </c>
+      <c r="C534" t="n">
+        <v>391</v>
+      </c>
+      <c r="D534" t="n">
+        <v>0</v>
+      </c>
+      <c r="E534" t="n">
+        <v>0</v>
+      </c>
+      <c r="F534" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" s="1" t="inlineStr">
+        <is>
+          <t>07/set/2021</t>
+        </is>
+      </c>
+      <c r="B535" t="n">
+        <v>17366</v>
+      </c>
+      <c r="C535" t="n">
+        <v>392</v>
+      </c>
+      <c r="D535" t="n">
+        <v>1</v>
+      </c>
+      <c r="E535" t="n">
+        <v>40</v>
+      </c>
+      <c r="F535" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" s="1" t="inlineStr">
+        <is>
+          <t>08/set/2021</t>
+        </is>
+      </c>
+      <c r="B536" t="n">
+        <v>17366</v>
+      </c>
+      <c r="C536" t="n">
+        <v>392</v>
+      </c>
+      <c r="D536" t="n">
+        <v>0</v>
+      </c>
+      <c r="E536" t="n">
+        <v>0</v>
+      </c>
+      <c r="F536" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" s="1" t="inlineStr">
+        <is>
+          <t>09/set/2021</t>
+        </is>
+      </c>
+      <c r="B537" t="n">
+        <v>17366</v>
+      </c>
+      <c r="C537" t="n">
+        <v>392</v>
+      </c>
+      <c r="D537" t="n">
+        <v>0</v>
+      </c>
+      <c r="E537" t="n">
+        <v>0</v>
+      </c>
+      <c r="F537" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" s="1" t="inlineStr">
+        <is>
+          <t>10/set/2021</t>
+        </is>
+      </c>
+      <c r="B538" t="n">
+        <v>17366</v>
+      </c>
+      <c r="C538" t="n">
+        <v>392</v>
+      </c>
+      <c r="D538" t="n">
+        <v>0</v>
+      </c>
+      <c r="E538" t="n">
+        <v>0</v>
+      </c>
+      <c r="F538" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" s="1" t="inlineStr">
+        <is>
+          <t>11/set/2021</t>
+        </is>
+      </c>
+      <c r="B539" t="n">
+        <v>17366</v>
+      </c>
+      <c r="C539" t="n">
+        <v>392</v>
+      </c>
+      <c r="D539" t="n">
+        <v>0</v>
+      </c>
+      <c r="E539" t="n">
+        <v>0</v>
+      </c>
+      <c r="F539" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" s="1" t="inlineStr">
+        <is>
+          <t>12/set/2021</t>
+        </is>
+      </c>
+      <c r="B540" t="n">
+        <v>17366</v>
+      </c>
+      <c r="C540" t="n">
+        <v>392</v>
+      </c>
+      <c r="D540" t="n">
+        <v>0</v>
+      </c>
+      <c r="E540" t="n">
+        <v>0</v>
+      </c>
+      <c r="F540" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" s="1" t="inlineStr">
+        <is>
+          <t>13/set/2021</t>
+        </is>
+      </c>
+      <c r="B541" t="n">
+        <v>17387</v>
+      </c>
+      <c r="C541" t="n">
+        <v>392</v>
+      </c>
+      <c r="D541" t="n">
+        <v>0</v>
+      </c>
+      <c r="E541" t="n">
+        <v>21</v>
+      </c>
+      <c r="F541" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" s="1" t="inlineStr">
+        <is>
+          <t>14/set/2021</t>
+        </is>
+      </c>
+      <c r="B542" t="n">
+        <v>17387</v>
+      </c>
+      <c r="C542" t="n">
+        <v>392</v>
+      </c>
+      <c r="D542" t="n">
+        <v>0</v>
+      </c>
+      <c r="E542" t="n">
+        <v>0</v>
+      </c>
+      <c r="F542" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" s="1" t="inlineStr">
+        <is>
+          <t>15/set/2021</t>
+        </is>
+      </c>
+      <c r="B543" t="n">
+        <v>17397</v>
+      </c>
+      <c r="C543" t="n">
+        <v>392</v>
+      </c>
+      <c r="D543" t="n">
+        <v>0</v>
+      </c>
+      <c r="E543" t="n">
+        <v>10</v>
+      </c>
+      <c r="F543" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" s="1" t="inlineStr">
+        <is>
+          <t>16/set/2021</t>
+        </is>
+      </c>
+      <c r="B544" t="n">
+        <v>17397</v>
+      </c>
+      <c r="C544" t="n">
+        <v>392</v>
+      </c>
+      <c r="D544" t="n">
+        <v>0</v>
+      </c>
+      <c r="E544" t="n">
+        <v>0</v>
+      </c>
+      <c r="F544" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" s="1" t="inlineStr">
+        <is>
+          <t>17/set/2021</t>
+        </is>
+      </c>
+      <c r="B545" t="n">
+        <v>17397</v>
+      </c>
+      <c r="C545" t="n">
+        <v>392</v>
+      </c>
+      <c r="D545" t="n">
+        <v>0</v>
+      </c>
+      <c r="E545" t="n">
+        <v>0</v>
+      </c>
+      <c r="F545" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" s="1" t="inlineStr">
+        <is>
+          <t>18/set/2021</t>
+        </is>
+      </c>
+      <c r="B546" t="n">
+        <v>17397</v>
+      </c>
+      <c r="C546" t="n">
+        <v>392</v>
+      </c>
+      <c r="D546" t="n">
+        <v>0</v>
+      </c>
+      <c r="E546" t="n">
+        <v>0</v>
+      </c>
+      <c r="F546" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" s="1" t="inlineStr">
+        <is>
+          <t>19/set/2021</t>
+        </is>
+      </c>
+      <c r="B547" t="n">
+        <v>17397</v>
+      </c>
+      <c r="C547" t="n">
+        <v>392</v>
+      </c>
+      <c r="D547" t="n">
+        <v>0</v>
+      </c>
+      <c r="E547" t="n">
+        <v>0</v>
+      </c>
+      <c r="F547" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" s="1" t="inlineStr">
+        <is>
+          <t>20/set/2021</t>
+        </is>
+      </c>
+      <c r="B548" t="n">
+        <v>17397</v>
+      </c>
+      <c r="C548" t="n">
+        <v>392</v>
+      </c>
+      <c r="D548" t="n">
+        <v>0</v>
+      </c>
+      <c r="E548" t="n">
+        <v>0</v>
+      </c>
+      <c r="F548" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" s="1" t="inlineStr">
+        <is>
+          <t>21/set/2021</t>
+        </is>
+      </c>
+      <c r="B549" t="n">
+        <v>17397</v>
+      </c>
+      <c r="C549" t="n">
+        <v>392</v>
+      </c>
+      <c r="D549" t="n">
+        <v>0</v>
+      </c>
+      <c r="E549" t="n">
+        <v>0</v>
+      </c>
+      <c r="F549" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" s="1" t="inlineStr">
+        <is>
+          <t>22/set/2021</t>
+        </is>
+      </c>
+      <c r="B550" t="n">
+        <v>17397</v>
+      </c>
+      <c r="C550" t="n">
+        <v>392</v>
+      </c>
+      <c r="D550" t="n">
+        <v>0</v>
+      </c>
+      <c r="E550" t="n">
+        <v>0</v>
+      </c>
+      <c r="F550" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" s="1" t="inlineStr">
+        <is>
+          <t>23/set/2021</t>
+        </is>
+      </c>
+      <c r="B551" t="n">
+        <v>17397</v>
+      </c>
+      <c r="C551" t="n">
+        <v>392</v>
+      </c>
+      <c r="D551" t="n">
+        <v>0</v>
+      </c>
+      <c r="E551" t="n">
+        <v>0</v>
+      </c>
+      <c r="F551" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" s="1" t="inlineStr">
+        <is>
+          <t>24/set/2021</t>
+        </is>
+      </c>
+      <c r="B552" t="n">
+        <v>17397</v>
+      </c>
+      <c r="C552" t="n">
+        <v>392</v>
+      </c>
+      <c r="D552" t="n">
+        <v>0</v>
+      </c>
+      <c r="E552" t="n">
+        <v>0</v>
+      </c>
+      <c r="F552" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" s="1" t="inlineStr">
+        <is>
+          <t>25/set/2021</t>
+        </is>
+      </c>
+      <c r="B553" t="n">
+        <v>17397</v>
+      </c>
+      <c r="C553" t="n">
+        <v>392</v>
+      </c>
+      <c r="D553" t="n">
+        <v>0</v>
+      </c>
+      <c r="E553" t="n">
+        <v>0</v>
+      </c>
+      <c r="F553" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" s="1" t="inlineStr">
+        <is>
+          <t>26/set/2021</t>
+        </is>
+      </c>
+      <c r="B554" t="n">
+        <v>17397</v>
+      </c>
+      <c r="C554" t="n">
+        <v>392</v>
+      </c>
+      <c r="D554" t="n">
+        <v>0</v>
+      </c>
+      <c r="E554" t="n">
+        <v>0</v>
+      </c>
+      <c r="F554" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" s="1" t="inlineStr">
+        <is>
+          <t>27/set/2021</t>
+        </is>
+      </c>
+      <c r="B555" t="n">
+        <v>17397</v>
+      </c>
+      <c r="C555" t="n">
+        <v>392</v>
+      </c>
+      <c r="D555" t="n">
+        <v>0</v>
+      </c>
+      <c r="E555" t="n">
+        <v>0</v>
+      </c>
+      <c r="F555" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" s="1" t="inlineStr">
+        <is>
+          <t>28/set/2021</t>
+        </is>
+      </c>
+      <c r="B556" t="n">
+        <v>17397</v>
+      </c>
+      <c r="C556" t="n">
+        <v>392</v>
+      </c>
+      <c r="D556" t="n">
+        <v>0</v>
+      </c>
+      <c r="E556" t="n">
+        <v>0</v>
+      </c>
+      <c r="F556" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" s="1" t="inlineStr">
+        <is>
+          <t>29/set/2021</t>
+        </is>
+      </c>
+      <c r="B557" t="n">
+        <v>17397</v>
+      </c>
+      <c r="C557" t="n">
+        <v>392</v>
+      </c>
+      <c r="D557" t="n">
+        <v>0</v>
+      </c>
+      <c r="E557" t="n">
+        <v>0</v>
+      </c>
+      <c r="F557" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" s="1" t="inlineStr">
+        <is>
+          <t>30/set/2021</t>
+        </is>
+      </c>
+      <c r="B558" t="n">
+        <v>17397</v>
+      </c>
+      <c r="C558" t="n">
+        <v>392</v>
+      </c>
+      <c r="D558" t="n">
+        <v>0</v>
+      </c>
+      <c r="E558" t="n">
+        <v>0</v>
+      </c>
+      <c r="F558" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" s="1" t="inlineStr">
+        <is>
+          <t>01/out/2021</t>
+        </is>
+      </c>
+      <c r="B559" t="n">
+        <v>17397</v>
+      </c>
+      <c r="C559" t="n">
+        <v>392</v>
+      </c>
+      <c r="D559" t="n">
+        <v>0</v>
+      </c>
+      <c r="E559" t="n">
+        <v>0</v>
+      </c>
+      <c r="F559" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" s="1" t="inlineStr">
+        <is>
+          <t>02/out/2021</t>
+        </is>
+      </c>
+      <c r="B560" t="n">
+        <v>17397</v>
+      </c>
+      <c r="C560" t="n">
+        <v>392</v>
+      </c>
+      <c r="D560" t="n">
+        <v>0</v>
+      </c>
+      <c r="E560" t="n">
+        <v>0</v>
+      </c>
+      <c r="F560" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" s="1" t="inlineStr">
+        <is>
+          <t>03/out/2021</t>
+        </is>
+      </c>
+      <c r="B561" t="n">
+        <v>17397</v>
+      </c>
+      <c r="C561" t="n">
+        <v>392</v>
+      </c>
+      <c r="D561" t="n">
+        <v>0</v>
+      </c>
+      <c r="E561" t="n">
+        <v>0</v>
+      </c>
+      <c r="F561" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" s="1" t="inlineStr">
+        <is>
+          <t>04/out/2021</t>
+        </is>
+      </c>
+      <c r="B562" t="n">
+        <v>17397</v>
+      </c>
+      <c r="C562" t="n">
+        <v>392</v>
+      </c>
+      <c r="D562" t="n">
+        <v>0</v>
+      </c>
+      <c r="E562" t="n">
+        <v>0</v>
+      </c>
+      <c r="F562" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" s="1" t="inlineStr">
+        <is>
+          <t>05/out/2021</t>
+        </is>
+      </c>
+      <c r="B563" t="n">
+        <v>17541</v>
+      </c>
+      <c r="C563" t="n">
+        <v>393</v>
+      </c>
+      <c r="D563" t="n">
+        <v>1</v>
+      </c>
+      <c r="E563" t="n">
+        <v>144</v>
+      </c>
+      <c r="F563" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" s="1" t="inlineStr">
+        <is>
+          <t>06/out/2021</t>
+        </is>
+      </c>
+      <c r="B564" t="n">
+        <v>17551</v>
+      </c>
+      <c r="C564" t="n">
+        <v>393</v>
+      </c>
+      <c r="D564" t="n">
+        <v>0</v>
+      </c>
+      <c r="E564" t="n">
+        <v>10</v>
+      </c>
+      <c r="F564" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" s="1" t="inlineStr">
+        <is>
+          <t>07/out/2021</t>
+        </is>
+      </c>
+      <c r="B565" t="n">
+        <v>17561</v>
+      </c>
+      <c r="C565" t="n">
+        <v>393</v>
+      </c>
+      <c r="D565" t="n">
+        <v>0</v>
+      </c>
+      <c r="E565" t="n">
+        <v>10</v>
+      </c>
+      <c r="F565" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" s="1" t="inlineStr">
+        <is>
+          <t>08/out/2021</t>
+        </is>
+      </c>
+      <c r="B566" t="n">
+        <v>17561</v>
+      </c>
+      <c r="C566" t="n">
+        <v>393</v>
+      </c>
+      <c r="D566" t="n">
+        <v>0</v>
+      </c>
+      <c r="E566" t="n">
+        <v>0</v>
+      </c>
+      <c r="F566" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" s="1" t="inlineStr">
+        <is>
+          <t>09/out/2021</t>
+        </is>
+      </c>
+      <c r="B567" t="n">
+        <v>17561</v>
+      </c>
+      <c r="C567" t="n">
+        <v>393</v>
+      </c>
+      <c r="D567" t="n">
+        <v>0</v>
+      </c>
+      <c r="E567" t="n">
+        <v>0</v>
+      </c>
+      <c r="F567" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" s="1" t="inlineStr">
+        <is>
+          <t>10/out/2021</t>
+        </is>
+      </c>
+      <c r="B568" t="n">
+        <v>17582</v>
+      </c>
+      <c r="C568" t="n">
+        <v>393</v>
+      </c>
+      <c r="D568" t="n">
+        <v>0</v>
+      </c>
+      <c r="E568" t="n">
+        <v>21</v>
+      </c>
+      <c r="F568" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" s="1" t="inlineStr">
+        <is>
+          <t>11/out/2021</t>
+        </is>
+      </c>
+      <c r="B569" t="n">
+        <v>17588</v>
+      </c>
+      <c r="C569" t="n">
+        <v>393</v>
+      </c>
+      <c r="D569" t="n">
+        <v>0</v>
+      </c>
+      <c r="E569" t="n">
+        <v>6</v>
+      </c>
+      <c r="F569" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" s="1" t="inlineStr">
+        <is>
+          <t>12/out/2021</t>
+        </is>
+      </c>
+      <c r="B570" t="n">
+        <v>17588</v>
+      </c>
+      <c r="C570" t="n">
+        <v>393</v>
+      </c>
+      <c r="D570" t="n">
+        <v>0</v>
+      </c>
+      <c r="E570" t="n">
+        <v>0</v>
+      </c>
+      <c r="F570" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" s="1" t="inlineStr">
+        <is>
+          <t>13/out/2021</t>
+        </is>
+      </c>
+      <c r="B571" t="n">
+        <v>17588</v>
+      </c>
+      <c r="C571" t="n">
+        <v>393</v>
+      </c>
+      <c r="D571" t="n">
+        <v>0</v>
+      </c>
+      <c r="E571" t="n">
+        <v>0</v>
+      </c>
+      <c r="F571" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" s="1" t="inlineStr">
+        <is>
+          <t>14/out/2021</t>
+        </is>
+      </c>
+      <c r="B572" t="n">
+        <v>17612</v>
+      </c>
+      <c r="C572" t="n">
+        <v>393</v>
+      </c>
+      <c r="D572" t="n">
+        <v>0</v>
+      </c>
+      <c r="E572" t="n">
+        <v>24</v>
+      </c>
+      <c r="F572" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" s="1" t="inlineStr">
+        <is>
+          <t>15/out/2021</t>
+        </is>
+      </c>
+      <c r="B573" t="n">
+        <v>17612</v>
+      </c>
+      <c r="C573" t="n">
+        <v>393</v>
+      </c>
+      <c r="D573" t="n">
+        <v>0</v>
+      </c>
+      <c r="E573" t="n">
+        <v>0</v>
+      </c>
+      <c r="F573" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" s="1" t="inlineStr">
+        <is>
+          <t>16/out/2021</t>
+        </is>
+      </c>
+      <c r="B574" t="n">
+        <v>17612</v>
+      </c>
+      <c r="C574" t="n">
+        <v>393</v>
+      </c>
+      <c r="D574" t="n">
+        <v>0</v>
+      </c>
+      <c r="E574" t="n">
+        <v>0</v>
+      </c>
+      <c r="F574" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" s="1" t="inlineStr">
+        <is>
+          <t>17/out/2021</t>
+        </is>
+      </c>
+      <c r="B575" t="n">
+        <v>17612</v>
+      </c>
+      <c r="C575" t="n">
+        <v>393</v>
+      </c>
+      <c r="D575" t="n">
+        <v>0</v>
+      </c>
+      <c r="E575" t="n">
+        <v>0</v>
+      </c>
+      <c r="F575" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" s="1" t="inlineStr">
+        <is>
+          <t>18/out/2021</t>
+        </is>
+      </c>
+      <c r="B576" t="n">
+        <v>17657</v>
+      </c>
+      <c r="C576" t="n">
+        <v>393</v>
+      </c>
+      <c r="D576" t="n">
+        <v>0</v>
+      </c>
+      <c r="E576" t="n">
+        <v>45</v>
+      </c>
+      <c r="F576" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" s="1" t="inlineStr">
+        <is>
+          <t>19/out/2021</t>
+        </is>
+      </c>
+      <c r="B577" t="n">
+        <v>17668</v>
+      </c>
+      <c r="C577" t="n">
+        <v>393</v>
+      </c>
+      <c r="D577" t="n">
+        <v>0</v>
+      </c>
+      <c r="E577" t="n">
+        <v>11</v>
+      </c>
+      <c r="F577" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" s="1" t="inlineStr">
+        <is>
+          <t>20/out/2021</t>
+        </is>
+      </c>
+      <c r="B578" t="n">
+        <v>17679</v>
+      </c>
+      <c r="C578" t="n">
+        <v>393</v>
+      </c>
+      <c r="D578" t="n">
+        <v>0</v>
+      </c>
+      <c r="E578" t="n">
+        <v>11</v>
+      </c>
+      <c r="F578" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" s="1" t="inlineStr">
+        <is>
+          <t>21/out/2021</t>
+        </is>
+      </c>
+      <c r="B579" t="n">
+        <v>17701</v>
+      </c>
+      <c r="C579" t="n">
+        <v>393</v>
+      </c>
+      <c r="D579" t="n">
+        <v>0</v>
+      </c>
+      <c r="E579" t="n">
+        <v>22</v>
+      </c>
+      <c r="F579" t="n">
+        <v>218162</v>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" s="1" t="inlineStr">
+        <is>
+          <t>22/out/2021</t>
+        </is>
+      </c>
+      <c r="B580" t="n">
+        <v>17701</v>
+      </c>
+      <c r="C580" t="n">
+        <v>393</v>
+      </c>
+      <c r="D580" t="n">
+        <v>0</v>
+      </c>
+      <c r="E580" t="n">
+        <v>0</v>
+      </c>
+      <c r="F580" t="n">
+        <v>218162</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>